<commit_message>
Updated the data files to reflect LGA names from VIC Parks Dataset
</commit_message>
<xml_diff>
--- a/data/LGA_ABS_data_21_22.xlsx
+++ b/data/LGA_ABS_data_21_22.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26529"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
   <workbookPr updateLinks="never" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="S:\erp2022 - final rebased\3218.0\2021-22\datacubes &amp; spreadsheets\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\anups\Desktop\Data Analytics\Homework\Group-Project-1\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CBA98819-B8D8-49EE-89B9-C8ACB352B56A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{63019B28-6E88-4A64-8EDC-9246B6480592}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2025" yWindow="3390" windowWidth="26985" windowHeight="15285" tabRatio="622" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="622" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Contents" sheetId="7" r:id="rId1"/>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="777" uniqueCount="615">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="777" uniqueCount="614">
   <si>
     <t>TOTAL QUEENSLAND</t>
   </si>
@@ -551,9 +551,6 @@
     <t>Baw Baw</t>
   </si>
   <si>
-    <t>Bayside (Vic.)</t>
-  </si>
-  <si>
     <t>Benalla</t>
   </si>
   <si>
@@ -635,15 +632,9 @@
     <t>Indigo</t>
   </si>
   <si>
-    <t>Kingston (Vic.)</t>
-  </si>
-  <si>
     <t>Knox</t>
   </si>
   <si>
-    <t>Latrobe (Vic.)</t>
-  </si>
-  <si>
     <t>Loddon</t>
   </si>
   <si>
@@ -687,9 +678,6 @@
   </si>
   <si>
     <t>Moreland</t>
-  </si>
-  <si>
-    <t>Mornington Peninsula</t>
   </si>
   <si>
     <t>Mount Alexander</t>
@@ -1944,6 +1932,15 @@
   </si>
   <si>
     <t>Estimated resident population and components, States and Territories, Australia</t>
+  </si>
+  <si>
+    <t>Bayside</t>
+  </si>
+  <si>
+    <t>Latrobe</t>
+  </si>
+  <si>
+    <t>Kingston</t>
   </si>
 </sst>
 </file>
@@ -3704,8 +3701,8 @@
   </sheetPr>
   <dimension ref="A1:F34"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
+    <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="3" topLeftCell="A86" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
@@ -3732,12 +3729,12 @@
     </row>
     <row r="2" spans="1:6" ht="20.100000000000001" customHeight="1">
       <c r="A2" s="4" t="s">
-        <v>573</v>
+        <v>569</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="12.75" customHeight="1">
       <c r="A3" s="95" t="s">
-        <v>608</v>
+        <v>604</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="12.75" customHeight="1">
@@ -3745,7 +3742,7 @@
     </row>
     <row r="5" spans="1:6" ht="12.75" customHeight="1">
       <c r="A5" s="34" t="s">
-        <v>609</v>
+        <v>605</v>
       </c>
       <c r="B5" s="25"/>
     </row>
@@ -3770,7 +3767,7 @@
         <v>1</v>
       </c>
       <c r="C9" s="42" t="s">
-        <v>593</v>
+        <v>589</v>
       </c>
     </row>
     <row r="10" spans="1:6" ht="12.75" customHeight="1">
@@ -3778,7 +3775,7 @@
         <v>2</v>
       </c>
       <c r="C10" s="38" t="s">
-        <v>594</v>
+        <v>590</v>
       </c>
     </row>
     <row r="11" spans="1:6" ht="12.75" customHeight="1">
@@ -3786,7 +3783,7 @@
         <v>3</v>
       </c>
       <c r="C11" s="38" t="s">
-        <v>595</v>
+        <v>591</v>
       </c>
     </row>
     <row r="12" spans="1:6" ht="12.75" customHeight="1">
@@ -3794,7 +3791,7 @@
         <v>4</v>
       </c>
       <c r="C12" s="38" t="s">
-        <v>596</v>
+        <v>592</v>
       </c>
     </row>
     <row r="13" spans="1:6" ht="12.75" customHeight="1">
@@ -3802,7 +3799,7 @@
         <v>5</v>
       </c>
       <c r="C13" s="38" t="s">
-        <v>597</v>
+        <v>593</v>
       </c>
     </row>
     <row r="14" spans="1:6" ht="12.75" customHeight="1">
@@ -3810,7 +3807,7 @@
         <v>6</v>
       </c>
       <c r="C14" s="38" t="s">
-        <v>598</v>
+        <v>594</v>
       </c>
     </row>
     <row r="15" spans="1:6" ht="12.75" customHeight="1">
@@ -3818,7 +3815,7 @@
         <v>7</v>
       </c>
       <c r="C15" s="38" t="s">
-        <v>599</v>
+        <v>595</v>
       </c>
     </row>
     <row r="16" spans="1:6" ht="12.75" customHeight="1">
@@ -3826,7 +3823,7 @@
         <v>8</v>
       </c>
       <c r="C16" s="38" t="s">
-        <v>614</v>
+        <v>610</v>
       </c>
     </row>
     <row r="17" spans="2:3" ht="12.75" customHeight="1">
@@ -3855,7 +3852,7 @@
     </row>
     <row r="22" spans="2:3" ht="12.75" customHeight="1">
       <c r="B22" s="1" t="s">
-        <v>573</v>
+        <v>569</v>
       </c>
       <c r="C22" s="9"/>
     </row>
@@ -3896,7 +3893,7 @@
     <row r="31" spans="2:3" ht="12.75" customHeight="1"/>
     <row r="32" spans="2:3" ht="12.75" customHeight="1">
       <c r="B32" s="101" t="s">
-        <v>574</v>
+        <v>570</v>
       </c>
       <c r="C32" s="101"/>
     </row>
@@ -4044,7 +4041,7 @@
     <row r="12" spans="1:6" ht="51" customHeight="1">
       <c r="A12" s="7"/>
       <c r="B12" s="96" t="s">
-        <v>611</v>
+        <v>607</v>
       </c>
     </row>
     <row r="13" spans="1:6" ht="12.75">
@@ -4054,7 +4051,7 @@
     <row r="14" spans="1:6" ht="25.5">
       <c r="A14" s="7"/>
       <c r="B14" s="97" t="s">
-        <v>612</v>
+        <v>608</v>
       </c>
     </row>
     <row r="15" spans="1:6" ht="12.75">
@@ -4064,7 +4061,7 @@
     <row r="16" spans="1:6" ht="25.5">
       <c r="A16" s="7"/>
       <c r="B16" s="99" t="s">
-        <v>613</v>
+        <v>609</v>
       </c>
     </row>
     <row r="17" spans="1:2" ht="12.75">
@@ -4074,7 +4071,7 @@
     <row r="18" spans="1:2" ht="25.5">
       <c r="A18" s="7"/>
       <c r="B18" s="97" t="s">
-        <v>610</v>
+        <v>606</v>
       </c>
     </row>
     <row r="19" spans="1:2" ht="12.75">
@@ -4186,7 +4183,7 @@
     </row>
     <row r="4" spans="1:14" s="23" customFormat="1" ht="20.100000000000001" customHeight="1">
       <c r="A4" s="1" t="s">
-        <v>600</v>
+        <v>596</v>
       </c>
       <c r="B4" s="62"/>
       <c r="C4" s="62"/>
@@ -4220,7 +4217,7 @@
       <c r="G6" s="102"/>
       <c r="H6" s="52"/>
       <c r="I6" s="105" t="s">
-        <v>575</v>
+        <v>571</v>
       </c>
       <c r="J6" s="105"/>
       <c r="K6" s="105"/>
@@ -4238,7 +4235,7 @@
       </c>
       <c r="E7" s="6"/>
       <c r="F7" s="103" t="s">
-        <v>592</v>
+        <v>588</v>
       </c>
       <c r="G7" s="104"/>
       <c r="H7" s="52"/>
@@ -4256,7 +4253,7 @@
         <v>6</v>
       </c>
       <c r="N7" s="29" t="s">
-        <v>576</v>
+        <v>572</v>
       </c>
     </row>
     <row r="8" spans="1:14" s="15" customFormat="1" ht="11.25" customHeight="1">
@@ -4356,7 +4353,7 @@
         <v>10180</v>
       </c>
       <c r="B11" s="16" t="s">
-        <v>578</v>
+        <v>574</v>
       </c>
       <c r="C11" s="84">
         <v>29332</v>
@@ -4470,7 +4467,7 @@
         <v>10470</v>
       </c>
       <c r="B14" s="16" t="s">
-        <v>579</v>
+        <v>575</v>
       </c>
       <c r="C14" s="84">
         <v>43674</v>
@@ -5572,7 +5569,7 @@
         <v>12160</v>
       </c>
       <c r="B43" s="16" t="s">
-        <v>580</v>
+        <v>576</v>
       </c>
       <c r="C43" s="84">
         <v>11390</v>
@@ -5686,7 +5683,7 @@
         <v>12390</v>
       </c>
       <c r="B46" s="16" t="s">
-        <v>581</v>
+        <v>577</v>
       </c>
       <c r="C46" s="84">
         <v>55528</v>
@@ -6104,7 +6101,7 @@
         <v>13340</v>
       </c>
       <c r="B57" s="16" t="s">
-        <v>582</v>
+        <v>578</v>
       </c>
       <c r="C57" s="84">
         <v>11109</v>
@@ -7130,7 +7127,7 @@
         <v>15270</v>
       </c>
       <c r="B84" s="16" t="s">
-        <v>583</v>
+        <v>579</v>
       </c>
       <c r="C84" s="84">
         <v>25714</v>
@@ -7890,7 +7887,7 @@
         <v>16490</v>
       </c>
       <c r="B104" s="16" t="s">
-        <v>584</v>
+        <v>580</v>
       </c>
       <c r="C104" s="84">
         <v>63404</v>
@@ -8156,7 +8153,7 @@
         <v>17040</v>
       </c>
       <c r="B111" s="16" t="s">
-        <v>585</v>
+        <v>581</v>
       </c>
       <c r="C111" s="84">
         <v>21667</v>
@@ -8270,7 +8267,7 @@
         <v>17150</v>
       </c>
       <c r="B114" s="16" t="s">
-        <v>586</v>
+        <v>582</v>
       </c>
       <c r="C114" s="84">
         <v>230994</v>
@@ -8346,7 +8343,7 @@
         <v>17310</v>
       </c>
       <c r="B116" s="16" t="s">
-        <v>587</v>
+        <v>583</v>
       </c>
       <c r="C116" s="84">
         <v>63670</v>
@@ -8460,7 +8457,7 @@
         <v>17420</v>
       </c>
       <c r="B119" s="16" t="s">
-        <v>588</v>
+        <v>584</v>
       </c>
       <c r="C119" s="84">
         <v>192660</v>
@@ -8536,7 +8533,7 @@
         <v>17620</v>
       </c>
       <c r="B121" s="16" t="s">
-        <v>589</v>
+        <v>585</v>
       </c>
       <c r="C121" s="84">
         <v>14258</v>
@@ -8574,7 +8571,7 @@
         <v>17640</v>
       </c>
       <c r="B122" s="16" t="s">
-        <v>590</v>
+        <v>586</v>
       </c>
       <c r="C122" s="84">
         <v>8494</v>
@@ -8802,7 +8799,7 @@
         <v>18020</v>
       </c>
       <c r="B128" s="16" t="s">
-        <v>591</v>
+        <v>587</v>
       </c>
       <c r="C128" s="84">
         <v>9256</v>
@@ -9298,7 +9295,7 @@
     </row>
     <row r="144" spans="1:14" s="15" customFormat="1">
       <c r="A144" s="40" t="s">
-        <v>577</v>
+        <v>573</v>
       </c>
       <c r="B144" s="60"/>
       <c r="C144" s="60"/>
@@ -9353,10 +9350,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:N97"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="8" topLeftCell="A9" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="8" topLeftCell="A27" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="A2" sqref="A2"/>
-      <selection pane="bottomLeft" activeCell="A9" sqref="A9"/>
+      <selection pane="bottomLeft" activeCell="B63" sqref="B63"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="11.25"/>
@@ -9399,7 +9396,7 @@
     </row>
     <row r="4" spans="1:14" s="23" customFormat="1" ht="20.100000000000001" customHeight="1">
       <c r="A4" s="1" t="s">
-        <v>601</v>
+        <v>597</v>
       </c>
       <c r="B4" s="62"/>
       <c r="C4" s="62"/>
@@ -9433,7 +9430,7 @@
       <c r="G6" s="102"/>
       <c r="H6" s="52"/>
       <c r="I6" s="105" t="s">
-        <v>575</v>
+        <v>571</v>
       </c>
       <c r="J6" s="105"/>
       <c r="K6" s="105"/>
@@ -9451,7 +9448,7 @@
       </c>
       <c r="E7" s="6"/>
       <c r="F7" s="103" t="s">
-        <v>592</v>
+        <v>588</v>
       </c>
       <c r="G7" s="104"/>
       <c r="H7" s="52"/>
@@ -9469,7 +9466,7 @@
         <v>6</v>
       </c>
       <c r="N7" s="29" t="s">
-        <v>576</v>
+        <v>572</v>
       </c>
     </row>
     <row r="8" spans="1:14" s="15" customFormat="1" ht="11.25" customHeight="1">
@@ -9759,7 +9756,7 @@
         <v>20910</v>
       </c>
       <c r="B16" s="16" t="s">
-        <v>164</v>
+        <v>611</v>
       </c>
       <c r="C16" s="84">
         <v>102328</v>
@@ -9797,7 +9794,7 @@
         <v>21010</v>
       </c>
       <c r="B17" s="16" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="C17" s="84">
         <v>14436</v>
@@ -9835,7 +9832,7 @@
         <v>21110</v>
       </c>
       <c r="B18" s="16" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="C18" s="84">
         <v>169789</v>
@@ -9873,7 +9870,7 @@
         <v>21180</v>
       </c>
       <c r="B19" s="16" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="C19" s="84">
         <v>196631</v>
@@ -9911,7 +9908,7 @@
         <v>21270</v>
       </c>
       <c r="B20" s="16" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="C20" s="84">
         <v>6132</v>
@@ -9949,7 +9946,7 @@
         <v>21370</v>
       </c>
       <c r="B21" s="16" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="C21" s="84">
         <v>38556</v>
@@ -9987,7 +9984,7 @@
         <v>21450</v>
       </c>
       <c r="B22" s="16" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="C22" s="84">
         <v>119573</v>
@@ -10025,7 +10022,7 @@
         <v>21610</v>
       </c>
       <c r="B23" s="16" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="C23" s="84">
         <v>369558</v>
@@ -10063,7 +10060,7 @@
         <v>21670</v>
       </c>
       <c r="B24" s="16" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="C24" s="84">
         <v>13388</v>
@@ -10101,7 +10098,7 @@
         <v>21750</v>
       </c>
       <c r="B25" s="16" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="C25" s="84">
         <v>22309</v>
@@ -10139,7 +10136,7 @@
         <v>21830</v>
       </c>
       <c r="B26" s="16" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="C26" s="84">
         <v>16030</v>
@@ -10177,7 +10174,7 @@
         <v>21890</v>
       </c>
       <c r="B27" s="16" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="C27" s="84">
         <v>150296</v>
@@ -10215,7 +10212,7 @@
         <v>22110</v>
       </c>
       <c r="B28" s="16" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="C28" s="84">
         <v>48477</v>
@@ -10253,7 +10250,7 @@
         <v>22170</v>
       </c>
       <c r="B29" s="16" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="C29" s="84">
         <v>140824</v>
@@ -10291,7 +10288,7 @@
         <v>22250</v>
       </c>
       <c r="B30" s="16" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="C30" s="84">
         <v>10615</v>
@@ -10329,7 +10326,7 @@
         <v>22310</v>
       </c>
       <c r="B31" s="16" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="C31" s="84">
         <v>150638</v>
@@ -10367,7 +10364,7 @@
         <v>22410</v>
       </c>
       <c r="B32" s="16" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="C32" s="84">
         <v>20058</v>
@@ -10405,7 +10402,7 @@
         <v>22490</v>
       </c>
       <c r="B33" s="16" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="C33" s="84">
         <v>24892</v>
@@ -10443,7 +10440,7 @@
         <v>22620</v>
       </c>
       <c r="B34" s="16" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="C34" s="84">
         <v>121272</v>
@@ -10481,7 +10478,7 @@
         <v>22670</v>
       </c>
       <c r="B35" s="16" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="C35" s="84">
         <v>160100</v>
@@ -10519,7 +10516,7 @@
         <v>22750</v>
       </c>
       <c r="B36" s="16" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="C36" s="84">
         <v>270932</v>
@@ -10557,7 +10554,7 @@
         <v>22830</v>
       </c>
       <c r="B37" s="16" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="C37" s="84">
         <v>68526</v>
@@ -10595,7 +10592,7 @@
         <v>22910</v>
       </c>
       <c r="B38" s="16" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="C38" s="84">
         <v>16485</v>
@@ -10633,7 +10630,7 @@
         <v>22980</v>
       </c>
       <c r="B39" s="16" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="C39" s="84">
         <v>5656</v>
@@ -10671,7 +10668,7 @@
         <v>23110</v>
       </c>
       <c r="B40" s="16" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="C40" s="84">
         <v>92267</v>
@@ -10709,7 +10706,7 @@
         <v>23190</v>
       </c>
       <c r="B41" s="16" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="C41" s="84">
         <v>20376</v>
@@ -10747,7 +10744,7 @@
         <v>23270</v>
       </c>
       <c r="B42" s="16" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="C42" s="84">
         <v>246920</v>
@@ -10785,7 +10782,7 @@
         <v>23350</v>
       </c>
       <c r="B43" s="16" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="C43" s="84">
         <v>17251</v>
@@ -10823,7 +10820,7 @@
         <v>23430</v>
       </c>
       <c r="B44" s="16" t="s">
-        <v>192</v>
+        <v>613</v>
       </c>
       <c r="C44" s="84">
         <v>159554</v>
@@ -10861,7 +10858,7 @@
         <v>23670</v>
       </c>
       <c r="B45" s="16" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="C45" s="84">
         <v>160481</v>
@@ -10899,7 +10896,7 @@
         <v>23810</v>
       </c>
       <c r="B46" s="16" t="s">
-        <v>194</v>
+        <v>612</v>
       </c>
       <c r="C46" s="84">
         <v>77117</v>
@@ -10937,7 +10934,7 @@
         <v>23940</v>
       </c>
       <c r="B47" s="16" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="C47" s="84">
         <v>7703</v>
@@ -10975,7 +10972,7 @@
         <v>24130</v>
       </c>
       <c r="B48" s="16" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="C48" s="84">
         <v>51599</v>
@@ -11013,7 +11010,7 @@
         <v>24210</v>
       </c>
       <c r="B49" s="16" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="C49" s="84">
         <v>125821</v>
@@ -11051,7 +11048,7 @@
         <v>24250</v>
       </c>
       <c r="B50" s="16" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="C50" s="84">
         <v>10121</v>
@@ -11089,7 +11086,7 @@
         <v>24330</v>
       </c>
       <c r="B51" s="16" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
       <c r="C51" s="84">
         <v>86385</v>
@@ -11127,7 +11124,7 @@
         <v>24410</v>
       </c>
       <c r="B52" s="16" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="C52" s="84">
         <v>116075</v>
@@ -11165,7 +11162,7 @@
         <v>24600</v>
       </c>
       <c r="B53" s="16" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="C53" s="84">
         <v>153110</v>
@@ -11203,7 +11200,7 @@
         <v>24650</v>
       </c>
       <c r="B54" s="16" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
       <c r="C54" s="84">
         <v>181346</v>
@@ -11241,7 +11238,7 @@
         <v>24780</v>
       </c>
       <c r="B55" s="16" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="C55" s="84">
         <v>56966</v>
@@ -11279,7 +11276,7 @@
         <v>24850</v>
       </c>
       <c r="B56" s="16" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
       <c r="C56" s="84">
         <v>49712</v>
@@ -11317,7 +11314,7 @@
         <v>24900</v>
       </c>
       <c r="B57" s="16" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="C57" s="84">
         <v>30367</v>
@@ -11355,7 +11352,7 @@
         <v>24970</v>
       </c>
       <c r="B58" s="16" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="C58" s="84">
         <v>192893</v>
@@ -11393,7 +11390,7 @@
         <v>25060</v>
       </c>
       <c r="B59" s="16" t="s">
-        <v>207</v>
+        <v>204</v>
       </c>
       <c r="C59" s="84">
         <v>122950</v>
@@ -11431,7 +11428,7 @@
         <v>25150</v>
       </c>
       <c r="B60" s="16" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="C60" s="84">
         <v>37910</v>
@@ -11469,7 +11466,7 @@
         <v>25250</v>
       </c>
       <c r="B61" s="16" t="s">
-        <v>209</v>
+        <v>206</v>
       </c>
       <c r="C61" s="84">
         <v>173500</v>
@@ -11507,7 +11504,7 @@
         <v>25340</v>
       </c>
       <c r="B62" s="16" t="s">
-        <v>210</v>
+        <v>280</v>
       </c>
       <c r="C62" s="84">
         <v>170440</v>
@@ -11545,7 +11542,7 @@
         <v>25430</v>
       </c>
       <c r="B63" s="16" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="C63" s="84">
         <v>20114</v>
@@ -11583,7 +11580,7 @@
         <v>25490</v>
       </c>
       <c r="B64" s="16" t="s">
-        <v>212</v>
+        <v>208</v>
       </c>
       <c r="C64" s="84">
         <v>17296</v>
@@ -11621,7 +11618,7 @@
         <v>25620</v>
       </c>
       <c r="B65" s="16" t="s">
-        <v>213</v>
+        <v>209</v>
       </c>
       <c r="C65" s="84">
         <v>15139</v>
@@ -11659,7 +11656,7 @@
         <v>25710</v>
       </c>
       <c r="B66" s="16" t="s">
-        <v>214</v>
+        <v>210</v>
       </c>
       <c r="C66" s="84">
         <v>63450</v>
@@ -11697,7 +11694,7 @@
         <v>25810</v>
       </c>
       <c r="B67" s="16" t="s">
-        <v>215</v>
+        <v>211</v>
       </c>
       <c r="C67" s="84">
         <v>11886</v>
@@ -11735,7 +11732,7 @@
         <v>25900</v>
       </c>
       <c r="B68" s="16" t="s">
-        <v>216</v>
+        <v>212</v>
       </c>
       <c r="C68" s="84">
         <v>103438</v>
@@ -11773,7 +11770,7 @@
         <v>25990</v>
       </c>
       <c r="B69" s="16" t="s">
-        <v>217</v>
+        <v>213</v>
       </c>
       <c r="C69" s="84">
         <v>7619</v>
@@ -11811,7 +11808,7 @@
         <v>26080</v>
       </c>
       <c r="B70" s="16" t="s">
-        <v>218</v>
+        <v>214</v>
       </c>
       <c r="C70" s="84">
         <v>3236</v>
@@ -11849,7 +11846,7 @@
         <v>26170</v>
       </c>
       <c r="B71" s="16" t="s">
-        <v>219</v>
+        <v>215</v>
       </c>
       <c r="C71" s="84">
         <v>30388</v>
@@ -11887,7 +11884,7 @@
         <v>26260</v>
       </c>
       <c r="B72" s="16" t="s">
-        <v>220</v>
+        <v>216</v>
       </c>
       <c r="C72" s="84">
         <v>16492</v>
@@ -11925,7 +11922,7 @@
         <v>26350</v>
       </c>
       <c r="B73" s="16" t="s">
-        <v>221</v>
+        <v>217</v>
       </c>
       <c r="C73" s="84">
         <v>106190</v>
@@ -11963,7 +11960,7 @@
         <v>26430</v>
       </c>
       <c r="B74" s="16" t="s">
-        <v>222</v>
+        <v>218</v>
       </c>
       <c r="C74" s="84">
         <v>11368</v>
@@ -12001,7 +11998,7 @@
         <v>26490</v>
       </c>
       <c r="B75" s="16" t="s">
-        <v>223</v>
+        <v>219</v>
       </c>
       <c r="C75" s="84">
         <v>37648</v>
@@ -12039,7 +12036,7 @@
         <v>26610</v>
       </c>
       <c r="B76" s="16" t="s">
-        <v>224</v>
+        <v>220</v>
       </c>
       <c r="C76" s="84">
         <v>21381</v>
@@ -12077,7 +12074,7 @@
         <v>26670</v>
       </c>
       <c r="B77" s="16" t="s">
-        <v>225</v>
+        <v>221</v>
       </c>
       <c r="C77" s="84">
         <v>6186</v>
@@ -12115,7 +12112,7 @@
         <v>26700</v>
       </c>
       <c r="B78" s="16" t="s">
-        <v>226</v>
+        <v>222</v>
       </c>
       <c r="C78" s="84">
         <v>29751</v>
@@ -12153,7 +12150,7 @@
         <v>26730</v>
       </c>
       <c r="B79" s="16" t="s">
-        <v>227</v>
+        <v>223</v>
       </c>
       <c r="C79" s="84">
         <v>35433</v>
@@ -12191,7 +12188,7 @@
         <v>26810</v>
       </c>
       <c r="B80" s="16" t="s">
-        <v>228</v>
+        <v>224</v>
       </c>
       <c r="C80" s="84">
         <v>45469</v>
@@ -12229,7 +12226,7 @@
         <v>26890</v>
       </c>
       <c r="B81" s="16" t="s">
-        <v>229</v>
+        <v>225</v>
       </c>
       <c r="C81" s="84">
         <v>3978</v>
@@ -12267,7 +12264,7 @@
         <v>26980</v>
       </c>
       <c r="B82" s="16" t="s">
-        <v>230</v>
+        <v>226</v>
       </c>
       <c r="C82" s="84">
         <v>171077</v>
@@ -12305,7 +12302,7 @@
         <v>27070</v>
       </c>
       <c r="B83" s="16" t="s">
-        <v>231</v>
+        <v>227</v>
       </c>
       <c r="C83" s="84">
         <v>231831</v>
@@ -12343,7 +12340,7 @@
         <v>27170</v>
       </c>
       <c r="B84" s="16" t="s">
-        <v>232</v>
+        <v>228</v>
       </c>
       <c r="C84" s="84">
         <v>43207</v>
@@ -12381,7 +12378,7 @@
         <v>27260</v>
       </c>
       <c r="B85" s="16" t="s">
-        <v>233</v>
+        <v>229</v>
       </c>
       <c r="C85" s="84">
         <v>296322</v>
@@ -12419,7 +12416,7 @@
         <v>27350</v>
       </c>
       <c r="B86" s="16" t="s">
-        <v>234</v>
+        <v>230</v>
       </c>
       <c r="C86" s="84">
         <v>91521</v>
@@ -12457,7 +12454,7 @@
         <v>27450</v>
       </c>
       <c r="B87" s="16" t="s">
-        <v>235</v>
+        <v>231</v>
       </c>
       <c r="C87" s="84">
         <v>157421</v>
@@ -12495,7 +12492,7 @@
         <v>27630</v>
       </c>
       <c r="B88" s="16" t="s">
-        <v>236</v>
+        <v>232</v>
       </c>
       <c r="C88" s="84">
         <v>6510</v>
@@ -12649,7 +12646,7 @@
     </row>
     <row r="95" spans="1:14" s="15" customFormat="1">
       <c r="A95" s="40" t="s">
-        <v>577</v>
+        <v>573</v>
       </c>
       <c r="B95" s="60"/>
       <c r="C95" s="60"/>
@@ -12750,7 +12747,7 @@
     </row>
     <row r="4" spans="1:14" s="23" customFormat="1" ht="20.100000000000001" customHeight="1">
       <c r="A4" s="1" t="s">
-        <v>602</v>
+        <v>598</v>
       </c>
       <c r="B4" s="62"/>
       <c r="C4" s="62"/>
@@ -12784,7 +12781,7 @@
       <c r="G6" s="102"/>
       <c r="H6" s="52"/>
       <c r="I6" s="105" t="s">
-        <v>575</v>
+        <v>571</v>
       </c>
       <c r="J6" s="105"/>
       <c r="K6" s="105"/>
@@ -12802,7 +12799,7 @@
       </c>
       <c r="E7" s="6"/>
       <c r="F7" s="103" t="s">
-        <v>592</v>
+        <v>588</v>
       </c>
       <c r="G7" s="104"/>
       <c r="H7" s="52"/>
@@ -12820,7 +12817,7 @@
         <v>6</v>
       </c>
       <c r="N7" s="29" t="s">
-        <v>576</v>
+        <v>572</v>
       </c>
     </row>
     <row r="8" spans="1:14" s="15" customFormat="1" ht="11.25" customHeight="1">
@@ -12882,7 +12879,7 @@
         <v>30250</v>
       </c>
       <c r="B10" s="16" t="s">
-        <v>237</v>
+        <v>233</v>
       </c>
       <c r="C10" s="84">
         <v>1130</v>
@@ -12920,7 +12917,7 @@
         <v>30300</v>
       </c>
       <c r="B11" s="16" t="s">
-        <v>238</v>
+        <v>234</v>
       </c>
       <c r="C11" s="84">
         <v>4378</v>
@@ -12958,7 +12955,7 @@
         <v>30370</v>
       </c>
       <c r="B12" s="16" t="s">
-        <v>239</v>
+        <v>235</v>
       </c>
       <c r="C12" s="84">
         <v>14657</v>
@@ -12996,7 +12993,7 @@
         <v>30410</v>
       </c>
       <c r="B13" s="16" t="s">
-        <v>240</v>
+        <v>236</v>
       </c>
       <c r="C13" s="84">
         <v>2863</v>
@@ -13034,7 +13031,7 @@
         <v>30450</v>
       </c>
       <c r="B14" s="16" t="s">
-        <v>241</v>
+        <v>237</v>
       </c>
       <c r="C14" s="84">
         <v>312</v>
@@ -13072,7 +13069,7 @@
         <v>30760</v>
       </c>
       <c r="B15" s="16" t="s">
-        <v>242</v>
+        <v>238</v>
       </c>
       <c r="C15" s="84">
         <v>1918</v>
@@ -13110,7 +13107,7 @@
         <v>30900</v>
       </c>
       <c r="B16" s="16" t="s">
-        <v>243</v>
+        <v>239</v>
       </c>
       <c r="C16" s="84">
         <v>470</v>
@@ -13148,7 +13145,7 @@
         <v>31000</v>
       </c>
       <c r="B17" s="16" t="s">
-        <v>244</v>
+        <v>240</v>
       </c>
       <c r="C17" s="84">
         <v>1262968</v>
@@ -13186,7 +13183,7 @@
         <v>31750</v>
       </c>
       <c r="B18" s="16" t="s">
-        <v>245</v>
+        <v>241</v>
       </c>
       <c r="C18" s="84">
         <v>342</v>
@@ -13224,7 +13221,7 @@
         <v>31820</v>
       </c>
       <c r="B19" s="16" t="s">
-        <v>246</v>
+        <v>242</v>
       </c>
       <c r="C19" s="84">
         <v>100095</v>
@@ -13262,7 +13259,7 @@
         <v>31900</v>
       </c>
       <c r="B20" s="16" t="s">
-        <v>247</v>
+        <v>243</v>
       </c>
       <c r="C20" s="84">
         <v>16836</v>
@@ -13300,7 +13297,7 @@
         <v>31950</v>
       </c>
       <c r="B21" s="16" t="s">
-        <v>248</v>
+        <v>244</v>
       </c>
       <c r="C21" s="84">
         <v>430</v>
@@ -13338,7 +13335,7 @@
         <v>32080</v>
       </c>
       <c r="B22" s="16" t="s">
-        <v>249</v>
+        <v>245</v>
       </c>
       <c r="C22" s="84">
         <v>169250</v>
@@ -13376,7 +13373,7 @@
         <v>32250</v>
       </c>
       <c r="B23" s="16" t="s">
-        <v>250</v>
+        <v>246</v>
       </c>
       <c r="C23" s="84">
         <v>2158</v>
@@ -13414,7 +13411,7 @@
         <v>32260</v>
       </c>
       <c r="B24" s="16" t="s">
-        <v>251</v>
+        <v>247</v>
       </c>
       <c r="C24" s="84">
         <v>29511</v>
@@ -13452,7 +13449,7 @@
         <v>32270</v>
       </c>
       <c r="B25" s="16" t="s">
-        <v>252</v>
+        <v>248</v>
       </c>
       <c r="C25" s="84">
         <v>28298</v>
@@ -13490,7 +13487,7 @@
         <v>32310</v>
       </c>
       <c r="B26" s="16" t="s">
-        <v>253</v>
+        <v>249</v>
       </c>
       <c r="C26" s="84">
         <v>11920</v>
@@ -13528,7 +13525,7 @@
         <v>32330</v>
       </c>
       <c r="B27" s="16" t="s">
-        <v>254</v>
+        <v>250</v>
       </c>
       <c r="C27" s="84">
         <v>1211</v>
@@ -13566,7 +13563,7 @@
         <v>32450</v>
       </c>
       <c r="B28" s="16" t="s">
-        <v>255</v>
+        <v>251</v>
       </c>
       <c r="C28" s="84">
         <v>3704</v>
@@ -13604,7 +13601,7 @@
         <v>32500</v>
       </c>
       <c r="B29" s="16" t="s">
-        <v>256</v>
+        <v>252</v>
       </c>
       <c r="C29" s="84">
         <v>4631</v>
@@ -13642,7 +13639,7 @@
         <v>32600</v>
       </c>
       <c r="B30" s="16" t="s">
-        <v>257</v>
+        <v>253</v>
       </c>
       <c r="C30" s="84">
         <v>269</v>
@@ -13680,7 +13677,7 @@
         <v>32750</v>
       </c>
       <c r="B31" s="16" t="s">
-        <v>258</v>
+        <v>254</v>
       </c>
       <c r="C31" s="84">
         <v>270</v>
@@ -13718,7 +13715,7 @@
         <v>32770</v>
       </c>
       <c r="B32" s="16" t="s">
-        <v>259</v>
+        <v>255</v>
       </c>
       <c r="C32" s="84">
         <v>1434</v>
@@ -13756,7 +13753,7 @@
         <v>32810</v>
       </c>
       <c r="B33" s="16" t="s">
-        <v>260</v>
+        <v>256</v>
       </c>
       <c r="C33" s="84">
         <v>12441</v>
@@ -13794,7 +13791,7 @@
         <v>33100</v>
       </c>
       <c r="B34" s="16" t="s">
-        <v>261</v>
+        <v>257</v>
       </c>
       <c r="C34" s="84">
         <v>724</v>
@@ -13832,7 +13829,7 @@
         <v>33200</v>
       </c>
       <c r="B35" s="16" t="s">
-        <v>262</v>
+        <v>258</v>
       </c>
       <c r="C35" s="84">
         <v>1521</v>
@@ -13870,7 +13867,7 @@
         <v>33220</v>
       </c>
       <c r="B36" s="16" t="s">
-        <v>263</v>
+        <v>259</v>
       </c>
       <c r="C36" s="84">
         <v>112070</v>
@@ -13908,7 +13905,7 @@
         <v>33360</v>
       </c>
       <c r="B37" s="16" t="s">
-        <v>264</v>
+        <v>260</v>
       </c>
       <c r="C37" s="84">
         <v>64275</v>
@@ -13946,7 +13943,7 @@
         <v>33430</v>
       </c>
       <c r="B38" s="16" t="s">
-        <v>265</v>
+        <v>261</v>
       </c>
       <c r="C38" s="84">
         <v>633598</v>
@@ -13984,7 +13981,7 @@
         <v>33610</v>
       </c>
       <c r="B39" s="16" t="s">
-        <v>266</v>
+        <v>262</v>
       </c>
       <c r="C39" s="84">
         <v>10400</v>
@@ -14022,7 +14019,7 @@
         <v>33620</v>
       </c>
       <c r="B40" s="16" t="s">
-        <v>267</v>
+        <v>263</v>
       </c>
       <c r="C40" s="84">
         <v>53851</v>
@@ -14060,7 +14057,7 @@
         <v>33800</v>
       </c>
       <c r="B41" s="16" t="s">
-        <v>268</v>
+        <v>264</v>
       </c>
       <c r="C41" s="84">
         <v>10990</v>
@@ -14098,7 +14095,7 @@
         <v>33830</v>
       </c>
       <c r="B42" s="16" t="s">
-        <v>269</v>
+        <v>265</v>
       </c>
       <c r="C42" s="84">
         <v>998</v>
@@ -14136,7 +14133,7 @@
         <v>33960</v>
       </c>
       <c r="B43" s="16" t="s">
-        <v>270</v>
+        <v>266</v>
       </c>
       <c r="C43" s="84">
         <v>233314</v>
@@ -14174,7 +14171,7 @@
         <v>33980</v>
       </c>
       <c r="B44" s="16" t="s">
-        <v>271</v>
+        <v>267</v>
       </c>
       <c r="C44" s="84">
         <v>22419</v>
@@ -14212,7 +14209,7 @@
         <v>34420</v>
       </c>
       <c r="B45" s="16" t="s">
-        <v>272</v>
+        <v>268</v>
       </c>
       <c r="C45" s="84">
         <v>1107</v>
@@ -14250,7 +14247,7 @@
         <v>34530</v>
       </c>
       <c r="B46" s="16" t="s">
-        <v>273</v>
+        <v>269</v>
       </c>
       <c r="C46" s="84">
         <v>39877</v>
@@ -14288,7 +14285,7 @@
         <v>34570</v>
       </c>
       <c r="B47" s="16" t="s">
-        <v>274</v>
+        <v>270</v>
       </c>
       <c r="C47" s="84">
         <v>653</v>
@@ -14326,7 +14323,7 @@
         <v>34580</v>
       </c>
       <c r="B48" s="16" t="s">
-        <v>275</v>
+        <v>271</v>
       </c>
       <c r="C48" s="84">
         <v>41750</v>
@@ -14364,7 +14361,7 @@
         <v>34590</v>
       </c>
       <c r="B49" s="16" t="s">
-        <v>276</v>
+        <v>272</v>
       </c>
       <c r="C49" s="84">
         <v>350673</v>
@@ -14402,7 +14399,7 @@
         <v>34710</v>
       </c>
       <c r="B50" s="16" t="s">
-        <v>277</v>
+        <v>273</v>
       </c>
       <c r="C50" s="84">
         <v>3691</v>
@@ -14440,7 +14437,7 @@
         <v>34770</v>
       </c>
       <c r="B51" s="16" t="s">
-        <v>278</v>
+        <v>274</v>
       </c>
       <c r="C51" s="84">
         <v>123148</v>
@@ -14478,7 +14475,7 @@
         <v>34800</v>
       </c>
       <c r="B52" s="16" t="s">
-        <v>279</v>
+        <v>275</v>
       </c>
       <c r="C52" s="84">
         <v>838</v>
@@ -14516,7 +14513,7 @@
         <v>34830</v>
       </c>
       <c r="B53" s="16" t="s">
-        <v>280</v>
+        <v>276</v>
       </c>
       <c r="C53" s="84">
         <v>442</v>
@@ -14554,7 +14551,7 @@
         <v>34860</v>
       </c>
       <c r="B54" s="16" t="s">
-        <v>281</v>
+        <v>277</v>
       </c>
       <c r="C54" s="84">
         <v>12957</v>
@@ -14592,7 +14589,7 @@
         <v>34880</v>
       </c>
       <c r="B55" s="16" t="s">
-        <v>282</v>
+        <v>278</v>
       </c>
       <c r="C55" s="84">
         <v>23171</v>
@@ -14630,7 +14627,7 @@
         <v>35010</v>
       </c>
       <c r="B56" s="16" t="s">
-        <v>283</v>
+        <v>279</v>
       </c>
       <c r="C56" s="84">
         <v>484353</v>
@@ -14668,7 +14665,7 @@
         <v>35250</v>
       </c>
       <c r="B57" s="16" t="s">
-        <v>284</v>
+        <v>280</v>
       </c>
       <c r="C57" s="84">
         <v>1060</v>
@@ -14706,7 +14703,7 @@
         <v>35300</v>
       </c>
       <c r="B58" s="16" t="s">
-        <v>285</v>
+        <v>281</v>
       </c>
       <c r="C58" s="84">
         <v>19217</v>
@@ -14744,7 +14741,7 @@
         <v>35600</v>
       </c>
       <c r="B59" s="16" t="s">
-        <v>286</v>
+        <v>282</v>
       </c>
       <c r="C59" s="84">
         <v>4009</v>
@@ -14782,7 +14779,7 @@
         <v>35670</v>
       </c>
       <c r="B60" s="16" t="s">
-        <v>287</v>
+        <v>283</v>
       </c>
       <c r="C60" s="84">
         <v>906</v>
@@ -14820,7 +14817,7 @@
         <v>35740</v>
       </c>
       <c r="B61" s="16" t="s">
-        <v>288</v>
+        <v>284</v>
       </c>
       <c r="C61" s="84">
         <v>56874</v>
@@ -14858,7 +14855,7 @@
         <v>35760</v>
       </c>
       <c r="B62" s="16" t="s">
-        <v>289</v>
+        <v>285</v>
       </c>
       <c r="C62" s="84">
         <v>10142</v>
@@ -14896,7 +14893,7 @@
         <v>35780</v>
       </c>
       <c r="B63" s="16" t="s">
-        <v>290</v>
+        <v>286</v>
       </c>
       <c r="C63" s="84">
         <v>2885</v>
@@ -14934,7 +14931,7 @@
         <v>35790</v>
       </c>
       <c r="B64" s="16" t="s">
-        <v>291</v>
+        <v>287</v>
       </c>
       <c r="C64" s="84">
         <v>2180</v>
@@ -14972,7 +14969,7 @@
         <v>35800</v>
       </c>
       <c r="B65" s="16" t="s">
-        <v>292</v>
+        <v>288</v>
       </c>
       <c r="C65" s="84">
         <v>1707</v>
@@ -15010,7 +15007,7 @@
         <v>36070</v>
       </c>
       <c r="B66" s="16" t="s">
-        <v>293</v>
+        <v>289</v>
       </c>
       <c r="C66" s="84">
         <v>632</v>
@@ -15048,7 +15045,7 @@
         <v>36150</v>
       </c>
       <c r="B67" s="16" t="s">
-        <v>294</v>
+        <v>290</v>
       </c>
       <c r="C67" s="84">
         <v>702</v>
@@ -15086,7 +15083,7 @@
         <v>36250</v>
       </c>
       <c r="B68" s="16" t="s">
-        <v>295</v>
+        <v>291</v>
       </c>
       <c r="C68" s="84">
         <v>161709</v>
@@ -15124,7 +15121,7 @@
         <v>36300</v>
       </c>
       <c r="B69" s="16" t="s">
-        <v>296</v>
+        <v>292</v>
       </c>
       <c r="C69" s="84">
         <v>769</v>
@@ -15162,7 +15159,7 @@
         <v>36370</v>
       </c>
       <c r="B70" s="16" t="s">
-        <v>297</v>
+        <v>293</v>
       </c>
       <c r="C70" s="84">
         <v>82882</v>
@@ -15200,7 +15197,7 @@
         <v>36510</v>
       </c>
       <c r="B71" s="16" t="s">
-        <v>298</v>
+        <v>294</v>
       </c>
       <c r="C71" s="84">
         <v>43592</v>
@@ -15238,7 +15235,7 @@
         <v>36580</v>
       </c>
       <c r="B72" s="16" t="s">
-        <v>299</v>
+        <v>295</v>
       </c>
       <c r="C72" s="84">
         <v>25388</v>
@@ -15276,7 +15273,7 @@
         <v>36630</v>
       </c>
       <c r="B73" s="16" t="s">
-        <v>300</v>
+        <v>296</v>
       </c>
       <c r="C73" s="84">
         <v>33323</v>
@@ -15314,7 +15311,7 @@
         <v>36660</v>
       </c>
       <c r="B74" s="16" t="s">
-        <v>301</v>
+        <v>297</v>
       </c>
       <c r="C74" s="84">
         <v>36637</v>
@@ -15352,7 +15349,7 @@
         <v>36720</v>
       </c>
       <c r="B75" s="16" t="s">
-        <v>302</v>
+        <v>298</v>
       </c>
       <c r="C75" s="84">
         <v>346634</v>
@@ -15390,7 +15387,7 @@
         <v>36820</v>
       </c>
       <c r="B76" s="16" t="s">
-        <v>303</v>
+        <v>299</v>
       </c>
       <c r="C76" s="84">
         <v>26488</v>
@@ -15428,7 +15425,7 @@
         <v>36910</v>
       </c>
       <c r="B77" s="16" t="s">
-        <v>304</v>
+        <v>300</v>
       </c>
       <c r="C77" s="84">
         <v>175255</v>
@@ -15466,7 +15463,7 @@
         <v>36950</v>
       </c>
       <c r="B78" s="16" t="s">
-        <v>305</v>
+        <v>301</v>
       </c>
       <c r="C78" s="84">
         <v>3532</v>
@@ -15504,7 +15501,7 @@
         <v>36960</v>
       </c>
       <c r="B79" s="16" t="s">
-        <v>306</v>
+        <v>302</v>
       </c>
       <c r="C79" s="84">
         <v>4294</v>
@@ -15542,7 +15539,7 @@
         <v>37010</v>
       </c>
       <c r="B80" s="16" t="s">
-        <v>307</v>
+        <v>303</v>
       </c>
       <c r="C80" s="84">
         <v>195457</v>
@@ -15580,7 +15577,7 @@
         <v>37300</v>
       </c>
       <c r="B81" s="16" t="s">
-        <v>308</v>
+        <v>304</v>
       </c>
       <c r="C81" s="84">
         <v>4177</v>
@@ -15618,7 +15615,7 @@
         <v>37310</v>
       </c>
       <c r="B82" s="16" t="s">
-        <v>309</v>
+        <v>305</v>
       </c>
       <c r="C82" s="84">
         <v>34351</v>
@@ -15656,7 +15653,7 @@
         <v>37340</v>
       </c>
       <c r="B83" s="16" t="s">
-        <v>310</v>
+        <v>306</v>
       </c>
       <c r="C83" s="84">
         <v>37642</v>
@@ -15694,7 +15691,7 @@
         <v>37400</v>
       </c>
       <c r="B84" s="16" t="s">
-        <v>311</v>
+        <v>307</v>
       </c>
       <c r="C84" s="84">
         <v>1133</v>
@@ -15732,7 +15729,7 @@
         <v>37550</v>
       </c>
       <c r="B85" s="16" t="s">
-        <v>312</v>
+        <v>308</v>
       </c>
       <c r="C85" s="84">
         <v>1040</v>
@@ -15770,7 +15767,7 @@
         <v>37570</v>
       </c>
       <c r="B86" s="16" t="s">
-        <v>313</v>
+        <v>309</v>
       </c>
       <c r="C86" s="84">
         <v>284</v>
@@ -15808,7 +15805,7 @@
         <v>37600</v>
       </c>
       <c r="B87" s="16" t="s">
-        <v>314</v>
+        <v>310</v>
       </c>
       <c r="C87" s="84">
         <v>2597</v>
@@ -15908,7 +15905,7 @@
     </row>
     <row r="92" spans="1:14" s="15" customFormat="1">
       <c r="A92" s="40" t="s">
-        <v>577</v>
+        <v>573</v>
       </c>
       <c r="B92" s="60"/>
       <c r="C92" s="60"/>
@@ -16009,7 +16006,7 @@
     </row>
     <row r="4" spans="1:14" s="23" customFormat="1" ht="20.100000000000001" customHeight="1">
       <c r="A4" s="1" t="s">
-        <v>603</v>
+        <v>599</v>
       </c>
       <c r="B4" s="62"/>
       <c r="C4" s="62"/>
@@ -16043,7 +16040,7 @@
       <c r="G6" s="102"/>
       <c r="H6" s="52"/>
       <c r="I6" s="105" t="s">
-        <v>575</v>
+        <v>571</v>
       </c>
       <c r="J6" s="105"/>
       <c r="K6" s="105"/>
@@ -16061,7 +16058,7 @@
       </c>
       <c r="E7" s="6"/>
       <c r="F7" s="103" t="s">
-        <v>592</v>
+        <v>588</v>
       </c>
       <c r="G7" s="104"/>
       <c r="H7" s="52"/>
@@ -16079,7 +16076,7 @@
         <v>6</v>
       </c>
       <c r="N7" s="29" t="s">
-        <v>576</v>
+        <v>572</v>
       </c>
     </row>
     <row r="8" spans="1:14" s="15" customFormat="1" ht="11.25" customHeight="1">
@@ -16141,7 +16138,7 @@
         <v>40070</v>
       </c>
       <c r="B10" s="16" t="s">
-        <v>315</v>
+        <v>311</v>
       </c>
       <c r="C10" s="84">
         <v>25522</v>
@@ -16179,7 +16176,7 @@
         <v>40120</v>
       </c>
       <c r="B11" s="16" t="s">
-        <v>316</v>
+        <v>312</v>
       </c>
       <c r="C11" s="84">
         <v>41237</v>
@@ -16217,7 +16214,7 @@
         <v>40150</v>
       </c>
       <c r="B12" s="16" t="s">
-        <v>317</v>
+        <v>313</v>
       </c>
       <c r="C12" s="84">
         <v>9975</v>
@@ -16255,7 +16252,7 @@
         <v>40220</v>
       </c>
       <c r="B13" s="16" t="s">
-        <v>318</v>
+        <v>314</v>
       </c>
       <c r="C13" s="84">
         <v>29257</v>
@@ -16293,7 +16290,7 @@
         <v>40250</v>
       </c>
       <c r="B14" s="16" t="s">
-        <v>319</v>
+        <v>315</v>
       </c>
       <c r="C14" s="84">
         <v>2554</v>
@@ -16331,7 +16328,7 @@
         <v>40310</v>
       </c>
       <c r="B15" s="16" t="s">
-        <v>320</v>
+        <v>316</v>
       </c>
       <c r="C15" s="84">
         <v>25565</v>
@@ -16369,7 +16366,7 @@
         <v>40430</v>
       </c>
       <c r="B16" s="16" t="s">
-        <v>321</v>
+        <v>317</v>
       </c>
       <c r="C16" s="84">
         <v>2675</v>
@@ -16407,7 +16404,7 @@
         <v>40520</v>
       </c>
       <c r="B17" s="16" t="s">
-        <v>322</v>
+        <v>318</v>
       </c>
       <c r="C17" s="84">
         <v>10741</v>
@@ -16445,7 +16442,7 @@
         <v>40700</v>
       </c>
       <c r="B18" s="16" t="s">
-        <v>323</v>
+        <v>319</v>
       </c>
       <c r="C18" s="84">
         <v>46425</v>
@@ -16483,7 +16480,7 @@
         <v>40910</v>
       </c>
       <c r="B19" s="16" t="s">
-        <v>324</v>
+        <v>320</v>
       </c>
       <c r="C19" s="84">
         <v>55456</v>
@@ -16521,7 +16518,7 @@
         <v>41010</v>
       </c>
       <c r="B20" s="16" t="s">
-        <v>325</v>
+        <v>321</v>
       </c>
       <c r="C20" s="84">
         <v>3651</v>
@@ -16559,7 +16556,7 @@
         <v>41060</v>
       </c>
       <c r="B21" s="16" t="s">
-        <v>326</v>
+        <v>322</v>
       </c>
       <c r="C21" s="84">
         <v>123105</v>
@@ -16597,7 +16594,7 @@
         <v>41140</v>
       </c>
       <c r="B22" s="16" t="s">
-        <v>327</v>
+        <v>323</v>
       </c>
       <c r="C22" s="84">
         <v>9363</v>
@@ -16635,7 +16632,7 @@
         <v>41190</v>
       </c>
       <c r="B23" s="16" t="s">
-        <v>328</v>
+        <v>324</v>
       </c>
       <c r="C23" s="84">
         <v>1775</v>
@@ -16673,7 +16670,7 @@
         <v>41330</v>
       </c>
       <c r="B24" s="16" t="s">
-        <v>329</v>
+        <v>325</v>
       </c>
       <c r="C24" s="84">
         <v>1622</v>
@@ -16711,7 +16708,7 @@
         <v>41560</v>
       </c>
       <c r="B25" s="16" t="s">
-        <v>330</v>
+        <v>326</v>
       </c>
       <c r="C25" s="84">
         <v>15338</v>
@@ -16749,7 +16746,7 @@
         <v>41750</v>
       </c>
       <c r="B26" s="16" t="s">
-        <v>331</v>
+        <v>327</v>
       </c>
       <c r="C26" s="84">
         <v>1038</v>
@@ -16787,7 +16784,7 @@
         <v>41830</v>
       </c>
       <c r="B27" s="16" t="s">
-        <v>332</v>
+        <v>328</v>
       </c>
       <c r="C27" s="84">
         <v>1686</v>
@@ -16825,7 +16822,7 @@
         <v>41960</v>
       </c>
       <c r="B28" s="16" t="s">
-        <v>333</v>
+        <v>329</v>
       </c>
       <c r="C28" s="84">
         <v>1322</v>
@@ -16863,7 +16860,7 @@
         <v>42030</v>
       </c>
       <c r="B29" s="16" t="s">
-        <v>334</v>
+        <v>330</v>
       </c>
       <c r="C29" s="84">
         <v>25300</v>
@@ -16901,7 +16898,7 @@
         <v>42110</v>
       </c>
       <c r="B30" s="16" t="s">
-        <v>335</v>
+        <v>331</v>
       </c>
       <c r="C30" s="84">
         <v>4138</v>
@@ -16939,7 +16936,7 @@
         <v>42250</v>
       </c>
       <c r="B31" s="16" t="s">
-        <v>336</v>
+        <v>332</v>
       </c>
       <c r="C31" s="84">
         <v>8862</v>
@@ -16977,7 +16974,7 @@
         <v>42600</v>
       </c>
       <c r="B32" s="16" t="s">
-        <v>337</v>
+        <v>333</v>
       </c>
       <c r="C32" s="84">
         <v>37857</v>
@@ -17015,7 +17012,7 @@
         <v>42750</v>
       </c>
       <c r="B33" s="16" t="s">
-        <v>338</v>
+        <v>334</v>
       </c>
       <c r="C33" s="84">
         <v>4999</v>
@@ -17053,7 +17050,7 @@
         <v>43080</v>
       </c>
       <c r="B34" s="16" t="s">
-        <v>339</v>
+        <v>335</v>
       </c>
       <c r="C34" s="84">
         <v>1024</v>
@@ -17091,7 +17088,7 @@
         <v>43220</v>
       </c>
       <c r="B35" s="16" t="s">
-        <v>340</v>
+        <v>336</v>
       </c>
       <c r="C35" s="84">
         <v>1053</v>
@@ -17129,7 +17126,7 @@
         <v>43360</v>
       </c>
       <c r="B36" s="16" t="s">
-        <v>341</v>
+        <v>337</v>
       </c>
       <c r="C36" s="84">
         <v>2375</v>
@@ -17167,7 +17164,7 @@
         <v>43650</v>
       </c>
       <c r="B37" s="16" t="s">
-        <v>342</v>
+        <v>338</v>
       </c>
       <c r="C37" s="84">
         <v>16083</v>
@@ -17205,7 +17202,7 @@
         <v>43710</v>
       </c>
       <c r="B38" s="16" t="s">
-        <v>343</v>
+        <v>339</v>
       </c>
       <c r="C38" s="84">
         <v>6058</v>
@@ -17243,7 +17240,7 @@
         <v>43790</v>
       </c>
       <c r="B39" s="16" t="s">
-        <v>344</v>
+        <v>340</v>
       </c>
       <c r="C39" s="84">
         <v>11921</v>
@@ -17281,7 +17278,7 @@
         <v>44000</v>
       </c>
       <c r="B40" s="16" t="s">
-        <v>345</v>
+        <v>341</v>
       </c>
       <c r="C40" s="84">
         <v>102</v>
@@ -17319,7 +17316,7 @@
         <v>44060</v>
       </c>
       <c r="B41" s="16" t="s">
-        <v>346</v>
+        <v>342</v>
       </c>
       <c r="C41" s="84">
         <v>95610</v>
@@ -17357,7 +17354,7 @@
         <v>44210</v>
       </c>
       <c r="B42" s="16" t="s">
-        <v>347</v>
+        <v>343</v>
       </c>
       <c r="C42" s="84">
         <v>9355</v>
@@ -17395,7 +17392,7 @@
         <v>44340</v>
       </c>
       <c r="B43" s="16" t="s">
-        <v>348</v>
+        <v>344</v>
       </c>
       <c r="C43" s="84">
         <v>68162</v>
@@ -17433,7 +17430,7 @@
         <v>44550</v>
       </c>
       <c r="B44" s="16" t="s">
-        <v>349</v>
+        <v>345</v>
       </c>
       <c r="C44" s="84">
         <v>39632</v>
@@ -17471,7 +17468,7 @@
         <v>44620</v>
       </c>
       <c r="B45" s="16" t="s">
-        <v>350</v>
+        <v>346</v>
       </c>
       <c r="C45" s="84">
         <v>27637</v>
@@ -17509,7 +17506,7 @@
         <v>44830</v>
       </c>
       <c r="B46" s="16" t="s">
-        <v>351</v>
+        <v>347</v>
       </c>
       <c r="C46" s="84">
         <v>2920</v>
@@ -17547,7 +17544,7 @@
         <v>45040</v>
       </c>
       <c r="B47" s="16" t="s">
-        <v>352</v>
+        <v>348</v>
       </c>
       <c r="C47" s="84">
         <v>22339</v>
@@ -17585,7 +17582,7 @@
         <v>45090</v>
       </c>
       <c r="B48" s="16" t="s">
-        <v>353</v>
+        <v>349</v>
       </c>
       <c r="C48" s="84">
         <v>8892</v>
@@ -17623,7 +17620,7 @@
         <v>45120</v>
       </c>
       <c r="B49" s="16" t="s">
-        <v>354</v>
+        <v>350</v>
       </c>
       <c r="C49" s="84">
         <v>4659</v>
@@ -17661,7 +17658,7 @@
         <v>45290</v>
       </c>
       <c r="B50" s="16" t="s">
-        <v>355</v>
+        <v>351</v>
       </c>
       <c r="C50" s="84">
         <v>37823</v>
@@ -17699,7 +17696,7 @@
         <v>45340</v>
       </c>
       <c r="B51" s="16" t="s">
-        <v>356</v>
+        <v>352</v>
       </c>
       <c r="C51" s="84">
         <v>176595</v>
@@ -17737,7 +17734,7 @@
         <v>45400</v>
       </c>
       <c r="B52" s="16" t="s">
-        <v>357</v>
+        <v>353</v>
       </c>
       <c r="C52" s="84">
         <v>891</v>
@@ -17775,7 +17772,7 @@
         <v>45540</v>
       </c>
       <c r="B53" s="16" t="s">
-        <v>358</v>
+        <v>354</v>
       </c>
       <c r="C53" s="84">
         <v>1668</v>
@@ -17813,7 +17810,7 @@
         <v>45680</v>
       </c>
       <c r="B54" s="16" t="s">
-        <v>359</v>
+        <v>355</v>
       </c>
       <c r="C54" s="84">
         <v>100556</v>
@@ -17851,7 +17848,7 @@
         <v>45890</v>
       </c>
       <c r="B55" s="16" t="s">
-        <v>360</v>
+        <v>356</v>
       </c>
       <c r="C55" s="84">
         <v>134131</v>
@@ -17889,7 +17886,7 @@
         <v>46090</v>
       </c>
       <c r="B56" s="16" t="s">
-        <v>361</v>
+        <v>357</v>
       </c>
       <c r="C56" s="84">
         <v>14448</v>
@@ -17927,7 +17924,7 @@
         <v>46300</v>
       </c>
       <c r="B57" s="16" t="s">
-        <v>362</v>
+        <v>358</v>
       </c>
       <c r="C57" s="84">
         <v>14879</v>
@@ -17965,7 +17962,7 @@
         <v>46450</v>
       </c>
       <c r="B58" s="16" t="s">
-        <v>363</v>
+        <v>359</v>
       </c>
       <c r="C58" s="84">
         <v>17747</v>
@@ -18003,7 +18000,7 @@
         <v>46510</v>
       </c>
       <c r="B59" s="16" t="s">
-        <v>364</v>
+        <v>360</v>
       </c>
       <c r="C59" s="84">
         <v>22487</v>
@@ -18041,7 +18038,7 @@
         <v>46670</v>
       </c>
       <c r="B60" s="16" t="s">
-        <v>365</v>
+        <v>361</v>
       </c>
       <c r="C60" s="84">
         <v>10007</v>
@@ -18079,7 +18076,7 @@
         <v>46860</v>
       </c>
       <c r="B61" s="16" t="s">
-        <v>366</v>
+        <v>362</v>
       </c>
       <c r="C61" s="84">
         <v>1568</v>
@@ -18117,7 +18114,7 @@
         <v>46970</v>
       </c>
       <c r="B62" s="16" t="s">
-        <v>367</v>
+        <v>363</v>
       </c>
       <c r="C62" s="84">
         <v>4109</v>
@@ -18155,7 +18152,7 @@
         <v>47140</v>
       </c>
       <c r="B63" s="16" t="s">
-        <v>368</v>
+        <v>364</v>
       </c>
       <c r="C63" s="84">
         <v>147521</v>
@@ -18193,7 +18190,7 @@
         <v>47290</v>
       </c>
       <c r="B64" s="16" t="s">
-        <v>369</v>
+        <v>365</v>
       </c>
       <c r="C64" s="84">
         <v>2026</v>
@@ -18231,7 +18228,7 @@
         <v>47490</v>
       </c>
       <c r="B65" s="16" t="s">
-        <v>370</v>
+        <v>366</v>
       </c>
       <c r="C65" s="84">
         <v>2241</v>
@@ -18269,7 +18266,7 @@
         <v>47630</v>
       </c>
       <c r="B66" s="16" t="s">
-        <v>371</v>
+        <v>367</v>
       </c>
       <c r="C66" s="84">
         <v>7070</v>
@@ -18307,7 +18304,7 @@
         <v>47700</v>
       </c>
       <c r="B67" s="16" t="s">
-        <v>372</v>
+        <v>368</v>
       </c>
       <c r="C67" s="84">
         <v>102044</v>
@@ -18345,7 +18342,7 @@
         <v>47800</v>
       </c>
       <c r="B68" s="16" t="s">
-        <v>373</v>
+        <v>369</v>
       </c>
       <c r="C68" s="84">
         <v>5599</v>
@@ -18383,7 +18380,7 @@
         <v>47910</v>
       </c>
       <c r="B69" s="16" t="s">
-        <v>374</v>
+        <v>370</v>
       </c>
       <c r="C69" s="84">
         <v>2875</v>
@@ -18421,7 +18418,7 @@
         <v>47980</v>
       </c>
       <c r="B70" s="16" t="s">
-        <v>375</v>
+        <v>371</v>
       </c>
       <c r="C70" s="84">
         <v>39061</v>
@@ -18459,7 +18456,7 @@
         <v>48050</v>
       </c>
       <c r="B71" s="16" t="s">
-        <v>376</v>
+        <v>372</v>
       </c>
       <c r="C71" s="84">
         <v>16429</v>
@@ -18497,7 +18494,7 @@
         <v>48130</v>
       </c>
       <c r="B72" s="16" t="s">
-        <v>377</v>
+        <v>373</v>
       </c>
       <c r="C72" s="84">
         <v>6925</v>
@@ -18535,7 +18532,7 @@
         <v>48260</v>
       </c>
       <c r="B73" s="16" t="s">
-        <v>378</v>
+        <v>374</v>
       </c>
       <c r="C73" s="84">
         <v>8086</v>
@@ -18573,7 +18570,7 @@
         <v>48340</v>
       </c>
       <c r="B74" s="16" t="s">
-        <v>379</v>
+        <v>375</v>
       </c>
       <c r="C74" s="84">
         <v>12127</v>
@@ -18611,7 +18608,7 @@
         <v>48410</v>
       </c>
       <c r="B75" s="16" t="s">
-        <v>380</v>
+        <v>376</v>
       </c>
       <c r="C75" s="84">
         <v>62425</v>
@@ -18649,7 +18646,7 @@
         <v>48540</v>
       </c>
       <c r="B76" s="16" t="s">
-        <v>381</v>
+        <v>377</v>
       </c>
       <c r="C76" s="84">
         <v>21954</v>
@@ -18687,7 +18684,7 @@
         <v>48640</v>
       </c>
       <c r="B77" s="16" t="s">
-        <v>382</v>
+        <v>378</v>
       </c>
       <c r="C77" s="84">
         <v>1163</v>
@@ -18725,7 +18722,7 @@
         <v>48750</v>
       </c>
       <c r="B78" s="16" t="s">
-        <v>383</v>
+        <v>379</v>
       </c>
       <c r="C78" s="84">
         <v>5931</v>
@@ -18763,7 +18760,7 @@
         <v>48830</v>
       </c>
       <c r="B79" s="16" t="s">
-        <v>384</v>
+        <v>380</v>
       </c>
       <c r="C79" s="84">
         <v>11830</v>
@@ -18917,7 +18914,7 @@
     </row>
     <row r="86" spans="1:14" s="15" customFormat="1">
       <c r="A86" s="40" t="s">
-        <v>577</v>
+        <v>573</v>
       </c>
       <c r="B86" s="60"/>
       <c r="C86" s="60"/>
@@ -19019,7 +19016,7 @@
     </row>
     <row r="4" spans="1:14" s="23" customFormat="1" ht="20.100000000000001" customHeight="1">
       <c r="A4" s="1" t="s">
-        <v>604</v>
+        <v>600</v>
       </c>
       <c r="B4" s="62"/>
       <c r="C4" s="62"/>
@@ -19053,7 +19050,7 @@
       <c r="G6" s="102"/>
       <c r="H6" s="52"/>
       <c r="I6" s="105" t="s">
-        <v>575</v>
+        <v>571</v>
       </c>
       <c r="J6" s="105"/>
       <c r="K6" s="105"/>
@@ -19071,7 +19068,7 @@
       </c>
       <c r="E7" s="6"/>
       <c r="F7" s="103" t="s">
-        <v>592</v>
+        <v>588</v>
       </c>
       <c r="G7" s="104"/>
       <c r="H7" s="52"/>
@@ -19089,7 +19086,7 @@
         <v>6</v>
       </c>
       <c r="N7" s="29" t="s">
-        <v>576</v>
+        <v>572</v>
       </c>
     </row>
     <row r="8" spans="1:14" s="15" customFormat="1" ht="11.25" customHeight="1">
@@ -19151,7 +19148,7 @@
         <v>50080</v>
       </c>
       <c r="B10" s="16" t="s">
-        <v>387</v>
+        <v>383</v>
       </c>
       <c r="C10" s="84">
         <v>40105</v>
@@ -19189,7 +19186,7 @@
         <v>50210</v>
       </c>
       <c r="B11" s="16" t="s">
-        <v>388</v>
+        <v>384</v>
       </c>
       <c r="C11" s="84">
         <v>97644</v>
@@ -19227,7 +19224,7 @@
         <v>50250</v>
       </c>
       <c r="B12" s="16" t="s">
-        <v>389</v>
+        <v>385</v>
       </c>
       <c r="C12" s="84">
         <v>7781</v>
@@ -19265,7 +19262,7 @@
         <v>50280</v>
       </c>
       <c r="B13" s="16" t="s">
-        <v>390</v>
+        <v>386</v>
       </c>
       <c r="C13" s="84">
         <v>17303</v>
@@ -19303,7 +19300,7 @@
         <v>50350</v>
       </c>
       <c r="B14" s="16" t="s">
-        <v>391</v>
+        <v>387</v>
       </c>
       <c r="C14" s="84">
         <v>16500</v>
@@ -19341,7 +19338,7 @@
         <v>50420</v>
       </c>
       <c r="B15" s="16" t="s">
-        <v>392</v>
+        <v>388</v>
       </c>
       <c r="C15" s="84">
         <v>71774</v>
@@ -19379,7 +19376,7 @@
         <v>50490</v>
       </c>
       <c r="B16" s="16" t="s">
-        <v>393</v>
+        <v>389</v>
       </c>
       <c r="C16" s="84">
         <v>43868</v>
@@ -19417,7 +19414,7 @@
         <v>50560</v>
       </c>
       <c r="B17" s="16" t="s">
-        <v>394</v>
+        <v>390</v>
       </c>
       <c r="C17" s="84">
         <v>1735</v>
@@ -19455,7 +19452,7 @@
         <v>50630</v>
       </c>
       <c r="B18" s="16" t="s">
-        <v>395</v>
+        <v>391</v>
       </c>
       <c r="C18" s="84">
         <v>1760</v>
@@ -19493,7 +19490,7 @@
         <v>50770</v>
       </c>
       <c r="B19" s="16" t="s">
-        <v>396</v>
+        <v>392</v>
       </c>
       <c r="C19" s="84">
         <v>1874</v>
@@ -19531,7 +19528,7 @@
         <v>50840</v>
       </c>
       <c r="B20" s="16" t="s">
-        <v>397</v>
+        <v>393</v>
       </c>
       <c r="C20" s="84">
         <v>5376</v>
@@ -19569,7 +19566,7 @@
         <v>50910</v>
       </c>
       <c r="B21" s="16" t="s">
-        <v>398</v>
+        <v>394</v>
       </c>
       <c r="C21" s="84">
         <v>961</v>
@@ -19607,7 +19604,7 @@
         <v>50980</v>
       </c>
       <c r="B22" s="16" t="s">
-        <v>399</v>
+        <v>395</v>
       </c>
       <c r="C22" s="84">
         <v>18204</v>
@@ -19645,7 +19642,7 @@
         <v>51080</v>
       </c>
       <c r="B23" s="16" t="s">
-        <v>400</v>
+        <v>396</v>
       </c>
       <c r="C23" s="84">
         <v>1089</v>
@@ -19683,7 +19680,7 @@
         <v>51120</v>
       </c>
       <c r="B24" s="16" t="s">
-        <v>401</v>
+        <v>397</v>
       </c>
       <c r="C24" s="84">
         <v>1016</v>
@@ -19721,7 +19718,7 @@
         <v>51190</v>
       </c>
       <c r="B25" s="16" t="s">
-        <v>402</v>
+        <v>398</v>
       </c>
       <c r="C25" s="84">
         <v>34137</v>
@@ -19759,7 +19756,7 @@
         <v>51260</v>
       </c>
       <c r="B26" s="16" t="s">
-        <v>403</v>
+        <v>399</v>
       </c>
       <c r="C26" s="84">
         <v>42009</v>
@@ -19797,7 +19794,7 @@
         <v>51310</v>
       </c>
       <c r="B27" s="16" t="s">
-        <v>404</v>
+        <v>400</v>
       </c>
       <c r="C27" s="84">
         <v>29822</v>
@@ -19835,7 +19832,7 @@
         <v>51330</v>
       </c>
       <c r="B28" s="16" t="s">
-        <v>405</v>
+        <v>401</v>
       </c>
       <c r="C28" s="84">
         <v>99306</v>
@@ -19873,7 +19870,7 @@
         <v>51400</v>
       </c>
       <c r="B29" s="16" t="s">
-        <v>406</v>
+        <v>402</v>
       </c>
       <c r="C29" s="84">
         <v>18776</v>
@@ -19911,7 +19908,7 @@
         <v>51470</v>
       </c>
       <c r="B30" s="16" t="s">
-        <v>407</v>
+        <v>403</v>
       </c>
       <c r="C30" s="84">
         <v>573</v>
@@ -19949,7 +19946,7 @@
         <v>51540</v>
       </c>
       <c r="B31" s="16" t="s">
-        <v>408</v>
+        <v>404</v>
       </c>
       <c r="C31" s="84">
         <v>5520</v>
@@ -19987,7 +19984,7 @@
         <v>51610</v>
       </c>
       <c r="B32" s="16" t="s">
-        <v>409</v>
+        <v>405</v>
       </c>
       <c r="C32" s="84">
         <v>1613</v>
@@ -20025,7 +20022,7 @@
         <v>51680</v>
       </c>
       <c r="B33" s="16" t="s">
-        <v>410</v>
+        <v>406</v>
       </c>
       <c r="C33" s="84">
         <v>6099</v>
@@ -20063,7 +20060,7 @@
         <v>51750</v>
       </c>
       <c r="B34" s="16" t="s">
-        <v>411</v>
+        <v>407</v>
       </c>
       <c r="C34" s="84">
         <v>11643</v>
@@ -20101,7 +20098,7 @@
         <v>51820</v>
       </c>
       <c r="B35" s="16" t="s">
-        <v>412</v>
+        <v>408</v>
       </c>
       <c r="C35" s="84">
         <v>122212</v>
@@ -20139,7 +20136,7 @@
         <v>51890</v>
       </c>
       <c r="B36" s="16" t="s">
-        <v>413</v>
+        <v>409</v>
       </c>
       <c r="C36" s="84">
         <v>9086</v>
@@ -20177,7 +20174,7 @@
         <v>51960</v>
       </c>
       <c r="B37" s="16" t="s">
-        <v>414</v>
+        <v>410</v>
       </c>
       <c r="C37" s="84">
         <v>3638</v>
@@ -20215,7 +20212,7 @@
         <v>52030</v>
       </c>
       <c r="B38" s="16" t="s">
-        <v>415</v>
+        <v>411</v>
       </c>
       <c r="C38" s="84">
         <v>1091</v>
@@ -20253,7 +20250,7 @@
         <v>52100</v>
       </c>
       <c r="B39" s="16" t="s">
-        <v>416</v>
+        <v>412</v>
       </c>
       <c r="C39" s="84">
         <v>1028</v>
@@ -20291,7 +20288,7 @@
         <v>52170</v>
       </c>
       <c r="B40" s="16" t="s">
-        <v>417</v>
+        <v>413</v>
       </c>
       <c r="C40" s="84">
         <v>8245</v>
@@ -20329,7 +20326,7 @@
         <v>52240</v>
       </c>
       <c r="B41" s="16" t="s">
-        <v>418</v>
+        <v>414</v>
       </c>
       <c r="C41" s="84">
         <v>1134</v>
@@ -20367,7 +20364,7 @@
         <v>52310</v>
       </c>
       <c r="B42" s="16" t="s">
-        <v>419</v>
+        <v>415</v>
       </c>
       <c r="C42" s="84">
         <v>927</v>
@@ -20405,7 +20402,7 @@
         <v>52380</v>
       </c>
       <c r="B43" s="16" t="s">
-        <v>420</v>
+        <v>416</v>
       </c>
       <c r="C43" s="84">
         <v>228</v>
@@ -20443,7 +20440,7 @@
         <v>52450</v>
       </c>
       <c r="B44" s="16" t="s">
-        <v>421</v>
+        <v>417</v>
       </c>
       <c r="C44" s="84">
         <v>1341</v>
@@ -20481,7 +20478,7 @@
         <v>52520</v>
       </c>
       <c r="B45" s="16" t="s">
-        <v>422</v>
+        <v>418</v>
       </c>
       <c r="C45" s="84">
         <v>1436</v>
@@ -20519,7 +20516,7 @@
         <v>52590</v>
       </c>
       <c r="B46" s="16" t="s">
-        <v>423</v>
+        <v>419</v>
       </c>
       <c r="C46" s="84">
         <v>3473</v>
@@ -20557,7 +20554,7 @@
         <v>52660</v>
       </c>
       <c r="B47" s="16" t="s">
-        <v>424</v>
+        <v>420</v>
       </c>
       <c r="C47" s="84">
         <v>15197</v>
@@ -20595,7 +20592,7 @@
         <v>52730</v>
       </c>
       <c r="B48" s="16" t="s">
-        <v>425</v>
+        <v>421</v>
       </c>
       <c r="C48" s="84">
         <v>6468</v>
@@ -20633,7 +20630,7 @@
         <v>52800</v>
       </c>
       <c r="B49" s="16" t="s">
-        <v>426</v>
+        <v>422</v>
       </c>
       <c r="C49" s="84">
         <v>8414</v>
@@ -20671,7 +20668,7 @@
         <v>52870</v>
       </c>
       <c r="B50" s="16" t="s">
-        <v>427</v>
+        <v>423</v>
       </c>
       <c r="C50" s="84">
         <v>6312</v>
@@ -20709,7 +20706,7 @@
         <v>52940</v>
       </c>
       <c r="B51" s="16" t="s">
-        <v>428</v>
+        <v>424</v>
       </c>
       <c r="C51" s="84">
         <v>733</v>
@@ -20747,7 +20744,7 @@
         <v>53010</v>
       </c>
       <c r="B52" s="16" t="s">
-        <v>429</v>
+        <v>425</v>
       </c>
       <c r="C52" s="84">
         <v>698</v>
@@ -20785,7 +20782,7 @@
         <v>53080</v>
       </c>
       <c r="B53" s="16" t="s">
-        <v>430</v>
+        <v>426</v>
       </c>
       <c r="C53" s="84">
         <v>699</v>
@@ -20823,7 +20820,7 @@
         <v>53150</v>
       </c>
       <c r="B54" s="16" t="s">
-        <v>431</v>
+        <v>427</v>
       </c>
       <c r="C54" s="84">
         <v>8064</v>
@@ -20861,7 +20858,7 @@
         <v>53220</v>
       </c>
       <c r="B55" s="16" t="s">
-        <v>432</v>
+        <v>428</v>
       </c>
       <c r="C55" s="84">
         <v>10378</v>
@@ -20899,7 +20896,7 @@
         <v>53290</v>
       </c>
       <c r="B56" s="16" t="s">
-        <v>433</v>
+        <v>429</v>
       </c>
       <c r="C56" s="84">
         <v>14396</v>
@@ -20937,7 +20934,7 @@
         <v>53360</v>
       </c>
       <c r="B57" s="16" t="s">
-        <v>434</v>
+        <v>430</v>
       </c>
       <c r="C57" s="84">
         <v>3202</v>
@@ -20975,7 +20972,7 @@
         <v>53430</v>
       </c>
       <c r="B58" s="16" t="s">
-        <v>435</v>
+        <v>431</v>
       </c>
       <c r="C58" s="84">
         <v>33112</v>
@@ -21013,7 +21010,7 @@
         <v>53570</v>
       </c>
       <c r="B59" s="16" t="s">
-        <v>436</v>
+        <v>432</v>
       </c>
       <c r="C59" s="84">
         <v>5751</v>
@@ -21051,7 +21048,7 @@
         <v>53640</v>
       </c>
       <c r="B60" s="16" t="s">
-        <v>437</v>
+        <v>433</v>
       </c>
       <c r="C60" s="84">
         <v>1260</v>
@@ -21089,7 +21086,7 @@
         <v>53710</v>
       </c>
       <c r="B61" s="16" t="s">
-        <v>438</v>
+        <v>434</v>
       </c>
       <c r="C61" s="84">
         <v>983</v>
@@ -21127,7 +21124,7 @@
         <v>53780</v>
       </c>
       <c r="B62" s="16" t="s">
-        <v>439</v>
+        <v>435</v>
       </c>
       <c r="C62" s="84">
         <v>131366</v>
@@ -21165,7 +21162,7 @@
         <v>53800</v>
       </c>
       <c r="B63" s="16" t="s">
-        <v>440</v>
+        <v>436</v>
       </c>
       <c r="C63" s="84">
         <v>41182</v>
@@ -21203,7 +21200,7 @@
         <v>53920</v>
       </c>
       <c r="B64" s="16" t="s">
-        <v>441</v>
+        <v>437</v>
       </c>
       <c r="C64" s="84">
         <v>4038</v>
@@ -21241,7 +21238,7 @@
         <v>53990</v>
       </c>
       <c r="B65" s="16" t="s">
-        <v>442</v>
+        <v>438</v>
       </c>
       <c r="C65" s="84">
         <v>29625</v>
@@ -21279,7 +21276,7 @@
         <v>54060</v>
       </c>
       <c r="B66" s="16" t="s">
-        <v>443</v>
+        <v>439</v>
       </c>
       <c r="C66" s="84">
         <v>3769</v>
@@ -21317,7 +21314,7 @@
         <v>54130</v>
       </c>
       <c r="B67" s="16" t="s">
-        <v>444</v>
+        <v>440</v>
       </c>
       <c r="C67" s="84">
         <v>1196</v>
@@ -21355,7 +21352,7 @@
         <v>54170</v>
       </c>
       <c r="B68" s="16" t="s">
-        <v>445</v>
+        <v>441</v>
       </c>
       <c r="C68" s="84">
         <v>165050</v>
@@ -21393,7 +21390,7 @@
         <v>54200</v>
       </c>
       <c r="B69" s="16" t="s">
-        <v>446</v>
+        <v>442</v>
       </c>
       <c r="C69" s="84">
         <v>60804</v>
@@ -21431,7 +21428,7 @@
         <v>54280</v>
       </c>
       <c r="B70" s="16" t="s">
-        <v>447</v>
+        <v>443</v>
       </c>
       <c r="C70" s="84">
         <v>30670</v>
@@ -21469,7 +21466,7 @@
         <v>54310</v>
       </c>
       <c r="B71" s="16" t="s">
-        <v>448</v>
+        <v>444</v>
       </c>
       <c r="C71" s="84">
         <v>23412</v>
@@ -21507,7 +21504,7 @@
         <v>54340</v>
       </c>
       <c r="B72" s="16" t="s">
-        <v>449</v>
+        <v>445</v>
       </c>
       <c r="C72" s="84">
         <v>4227</v>
@@ -21545,7 +21542,7 @@
         <v>54410</v>
       </c>
       <c r="B73" s="16" t="s">
-        <v>450</v>
+        <v>446</v>
       </c>
       <c r="C73" s="84">
         <v>1177</v>
@@ -21583,7 +21580,7 @@
         <v>54480</v>
       </c>
       <c r="B74" s="16" t="s">
-        <v>451</v>
+        <v>447</v>
       </c>
       <c r="C74" s="84">
         <v>506</v>
@@ -21621,7 +21618,7 @@
         <v>54550</v>
       </c>
       <c r="B75" s="16" t="s">
-        <v>452</v>
+        <v>448</v>
       </c>
       <c r="C75" s="84">
         <v>1963</v>
@@ -21659,7 +21656,7 @@
         <v>54620</v>
       </c>
       <c r="B76" s="16" t="s">
-        <v>453</v>
+        <v>449</v>
       </c>
       <c r="C76" s="84">
         <v>872</v>
@@ -21697,7 +21694,7 @@
         <v>54690</v>
       </c>
       <c r="B77" s="16" t="s">
-        <v>454</v>
+        <v>450</v>
       </c>
       <c r="C77" s="84">
         <v>373</v>
@@ -21735,7 +21732,7 @@
         <v>54760</v>
       </c>
       <c r="B78" s="16" t="s">
-        <v>455</v>
+        <v>451</v>
       </c>
       <c r="C78" s="84">
         <v>789</v>
@@ -21773,7 +21770,7 @@
         <v>54830</v>
       </c>
       <c r="B79" s="16" t="s">
-        <v>456</v>
+        <v>452</v>
       </c>
       <c r="C79" s="84">
         <v>47660</v>
@@ -21811,7 +21808,7 @@
         <v>54900</v>
       </c>
       <c r="B80" s="16" t="s">
-        <v>457</v>
+        <v>453</v>
       </c>
       <c r="C80" s="84">
         <v>1299</v>
@@ -21849,7 +21846,7 @@
         <v>54970</v>
       </c>
       <c r="B81" s="16" t="s">
-        <v>458</v>
+        <v>454</v>
       </c>
       <c r="C81" s="84">
         <v>1432</v>
@@ -21887,7 +21884,7 @@
         <v>55040</v>
       </c>
       <c r="B82" s="16" t="s">
-        <v>459</v>
+        <v>455</v>
       </c>
       <c r="C82" s="84">
         <v>1716</v>
@@ -21925,7 +21922,7 @@
         <v>55110</v>
       </c>
       <c r="B83" s="16" t="s">
-        <v>460</v>
+        <v>456</v>
       </c>
       <c r="C83" s="84">
         <v>93412</v>
@@ -21963,7 +21960,7 @@
         <v>55180</v>
       </c>
       <c r="B84" s="16" t="s">
-        <v>461</v>
+        <v>457</v>
       </c>
       <c r="C84" s="84">
         <v>9351</v>
@@ -22001,7 +21998,7 @@
         <v>55250</v>
       </c>
       <c r="B85" s="16" t="s">
-        <v>462</v>
+        <v>458</v>
       </c>
       <c r="C85" s="84">
         <v>1287</v>
@@ -22039,7 +22036,7 @@
         <v>55320</v>
       </c>
       <c r="B86" s="16" t="s">
-        <v>463</v>
+        <v>459</v>
       </c>
       <c r="C86" s="84">
         <v>106823</v>
@@ -22077,7 +22074,7 @@
         <v>55390</v>
       </c>
       <c r="B87" s="16" t="s">
-        <v>464</v>
+        <v>460</v>
       </c>
       <c r="C87" s="84">
         <v>569</v>
@@ -22115,7 +22112,7 @@
         <v>55460</v>
       </c>
       <c r="B88" s="16" t="s">
-        <v>465</v>
+        <v>461</v>
       </c>
       <c r="C88" s="84">
         <v>3221</v>
@@ -22153,7 +22150,7 @@
         <v>55530</v>
       </c>
       <c r="B89" s="16" t="s">
-        <v>466</v>
+        <v>462</v>
       </c>
       <c r="C89" s="84">
         <v>423</v>
@@ -22191,7 +22188,7 @@
         <v>55600</v>
       </c>
       <c r="B90" s="16" t="s">
-        <v>467</v>
+        <v>463</v>
       </c>
       <c r="C90" s="84">
         <v>2382</v>
@@ -22229,7 +22226,7 @@
         <v>55670</v>
       </c>
       <c r="B91" s="16" t="s">
-        <v>468</v>
+        <v>464</v>
       </c>
       <c r="C91" s="84">
         <v>669</v>
@@ -22267,7 +22264,7 @@
         <v>55740</v>
       </c>
       <c r="B92" s="16" t="s">
-        <v>469</v>
+        <v>465</v>
       </c>
       <c r="C92" s="84">
         <v>9478</v>
@@ -22305,7 +22302,7 @@
         <v>55810</v>
       </c>
       <c r="B93" s="16" t="s">
-        <v>470</v>
+        <v>466</v>
       </c>
       <c r="C93" s="84">
         <v>699</v>
@@ -22343,7 +22340,7 @@
         <v>55880</v>
       </c>
       <c r="B94" s="16" t="s">
-        <v>471</v>
+        <v>467</v>
       </c>
       <c r="C94" s="84">
         <v>467</v>
@@ -22381,7 +22378,7 @@
         <v>55950</v>
       </c>
       <c r="B95" s="16" t="s">
-        <v>472</v>
+        <v>468</v>
       </c>
       <c r="C95" s="84">
         <v>593</v>
@@ -22419,7 +22416,7 @@
         <v>56090</v>
       </c>
       <c r="B96" s="16" t="s">
-        <v>473</v>
+        <v>469</v>
       </c>
       <c r="C96" s="84">
         <v>40539</v>
@@ -22457,7 +22454,7 @@
         <v>56160</v>
       </c>
       <c r="B97" s="16" t="s">
-        <v>474</v>
+        <v>470</v>
       </c>
       <c r="C97" s="84">
         <v>108</v>
@@ -22495,7 +22492,7 @@
         <v>56230</v>
       </c>
       <c r="B98" s="16" t="s">
-        <v>475</v>
+        <v>471</v>
       </c>
       <c r="C98" s="84">
         <v>18639</v>
@@ -22533,7 +22530,7 @@
         <v>56300</v>
       </c>
       <c r="B99" s="16" t="s">
-        <v>476</v>
+        <v>472</v>
       </c>
       <c r="C99" s="84">
         <v>1575</v>
@@ -22571,7 +22568,7 @@
         <v>56370</v>
       </c>
       <c r="B100" s="16" t="s">
-        <v>477</v>
+        <v>473</v>
       </c>
       <c r="C100" s="84">
         <v>820</v>
@@ -22609,7 +22606,7 @@
         <v>56460</v>
       </c>
       <c r="B101" s="16" t="s">
-        <v>478</v>
+        <v>474</v>
       </c>
       <c r="C101" s="84">
         <v>4937</v>
@@ -22647,7 +22644,7 @@
         <v>56580</v>
       </c>
       <c r="B102" s="16" t="s">
-        <v>479</v>
+        <v>475</v>
       </c>
       <c r="C102" s="84">
         <v>22924</v>
@@ -22685,7 +22682,7 @@
         <v>56620</v>
       </c>
       <c r="B103" s="16" t="s">
-        <v>480</v>
+        <v>476</v>
       </c>
       <c r="C103" s="84">
         <v>1476</v>
@@ -22723,7 +22720,7 @@
         <v>56730</v>
       </c>
       <c r="B104" s="16" t="s">
-        <v>481</v>
+        <v>477</v>
       </c>
       <c r="C104" s="84">
         <v>11804</v>
@@ -22761,7 +22758,7 @@
         <v>56790</v>
       </c>
       <c r="B105" s="16" t="s">
-        <v>482</v>
+        <v>478</v>
       </c>
       <c r="C105" s="84">
         <v>3332</v>
@@ -22799,7 +22796,7 @@
         <v>56860</v>
       </c>
       <c r="B106" s="16" t="s">
-        <v>483</v>
+        <v>479</v>
       </c>
       <c r="C106" s="84">
         <v>263</v>
@@ -22837,7 +22834,7 @@
         <v>56930</v>
       </c>
       <c r="B107" s="16" t="s">
-        <v>484</v>
+        <v>480</v>
       </c>
       <c r="C107" s="84">
         <v>1638</v>
@@ -22875,7 +22872,7 @@
         <v>57000</v>
       </c>
       <c r="B108" s="16" t="s">
-        <v>485</v>
+        <v>481</v>
       </c>
       <c r="C108" s="84">
         <v>652</v>
@@ -22913,7 +22910,7 @@
         <v>57080</v>
       </c>
       <c r="B109" s="16" t="s">
-        <v>486</v>
+        <v>482</v>
       </c>
       <c r="C109" s="84">
         <v>29653</v>
@@ -22951,7 +22948,7 @@
         <v>57140</v>
       </c>
       <c r="B110" s="16" t="s">
-        <v>487</v>
+        <v>483</v>
       </c>
       <c r="C110" s="84">
         <v>1072</v>
@@ -22989,7 +22986,7 @@
         <v>57210</v>
       </c>
       <c r="B111" s="16" t="s">
-        <v>488</v>
+        <v>484</v>
       </c>
       <c r="C111" s="84">
         <v>5534</v>
@@ -23027,7 +23024,7 @@
         <v>57280</v>
       </c>
       <c r="B112" s="16" t="s">
-        <v>489</v>
+        <v>485</v>
       </c>
       <c r="C112" s="84">
         <v>16666</v>
@@ -23065,7 +23062,7 @@
         <v>57350</v>
       </c>
       <c r="B113" s="16" t="s">
-        <v>490</v>
+        <v>486</v>
       </c>
       <c r="C113" s="84">
         <v>981</v>
@@ -23103,7 +23100,7 @@
         <v>57420</v>
       </c>
       <c r="B114" s="16" t="s">
-        <v>491</v>
+        <v>487</v>
       </c>
       <c r="C114" s="84">
         <v>2157</v>
@@ -23141,7 +23138,7 @@
         <v>57490</v>
       </c>
       <c r="B115" s="16" t="s">
-        <v>492</v>
+        <v>488</v>
       </c>
       <c r="C115" s="84">
         <v>140584</v>
@@ -23179,7 +23176,7 @@
         <v>57630</v>
       </c>
       <c r="B116" s="16" t="s">
-        <v>493</v>
+        <v>489</v>
       </c>
       <c r="C116" s="84">
         <v>117</v>
@@ -23217,7 +23214,7 @@
         <v>57700</v>
       </c>
       <c r="B117" s="16" t="s">
-        <v>494</v>
+        <v>490</v>
       </c>
       <c r="C117" s="84">
         <v>33349</v>
@@ -23255,7 +23252,7 @@
         <v>57770</v>
       </c>
       <c r="B118" s="16" t="s">
-        <v>495</v>
+        <v>491</v>
       </c>
       <c r="C118" s="84">
         <v>1069</v>
@@ -23293,7 +23290,7 @@
         <v>57840</v>
       </c>
       <c r="B119" s="16" t="s">
-        <v>496</v>
+        <v>492</v>
       </c>
       <c r="C119" s="84">
         <v>44952</v>
@@ -23331,7 +23328,7 @@
         <v>57910</v>
       </c>
       <c r="B120" s="16" t="s">
-        <v>497</v>
+        <v>493</v>
       </c>
       <c r="C120" s="84">
         <v>234322</v>
@@ -23369,7 +23366,7 @@
         <v>57980</v>
       </c>
       <c r="B121" s="16" t="s">
-        <v>498</v>
+        <v>494</v>
       </c>
       <c r="C121" s="84">
         <v>17902</v>
@@ -23407,7 +23404,7 @@
         <v>58050</v>
       </c>
       <c r="B122" s="16" t="s">
-        <v>499</v>
+        <v>495</v>
       </c>
       <c r="C122" s="84">
         <v>158689</v>
@@ -23445,7 +23442,7 @@
         <v>58190</v>
       </c>
       <c r="B123" s="16" t="s">
-        <v>500</v>
+        <v>496</v>
       </c>
       <c r="C123" s="84">
         <v>401</v>
@@ -23483,7 +23480,7 @@
         <v>58260</v>
       </c>
       <c r="B124" s="16" t="s">
-        <v>501</v>
+        <v>497</v>
       </c>
       <c r="C124" s="84">
         <v>586</v>
@@ -23521,7 +23518,7 @@
         <v>58330</v>
       </c>
       <c r="B125" s="16" t="s">
-        <v>502</v>
+        <v>498</v>
       </c>
       <c r="C125" s="84">
         <v>4709</v>
@@ -23559,7 +23556,7 @@
         <v>58400</v>
       </c>
       <c r="B126" s="16" t="s">
-        <v>503</v>
+        <v>499</v>
       </c>
       <c r="C126" s="84">
         <v>307</v>
@@ -23597,7 +23594,7 @@
         <v>58470</v>
       </c>
       <c r="B127" s="16" t="s">
-        <v>504</v>
+        <v>500</v>
       </c>
       <c r="C127" s="84">
         <v>180</v>
@@ -23635,7 +23632,7 @@
         <v>58510</v>
       </c>
       <c r="B128" s="16" t="s">
-        <v>505</v>
+        <v>501</v>
       </c>
       <c r="C128" s="84">
         <v>38296</v>
@@ -23673,7 +23670,7 @@
         <v>58540</v>
       </c>
       <c r="B129" s="16" t="s">
-        <v>506</v>
+        <v>502</v>
       </c>
       <c r="C129" s="84">
         <v>832</v>
@@ -23711,7 +23708,7 @@
         <v>58570</v>
       </c>
       <c r="B130" s="16" t="s">
-        <v>507</v>
+        <v>503</v>
       </c>
       <c r="C130" s="84">
         <v>37833</v>
@@ -23749,7 +23746,7 @@
         <v>58610</v>
       </c>
       <c r="B131" s="16" t="s">
-        <v>508</v>
+        <v>504</v>
       </c>
       <c r="C131" s="84">
         <v>1802</v>
@@ -23787,7 +23784,7 @@
         <v>58680</v>
       </c>
       <c r="B132" s="16" t="s">
-        <v>509</v>
+        <v>505</v>
       </c>
       <c r="C132" s="84">
         <v>551</v>
@@ -23825,7 +23822,7 @@
         <v>58760</v>
       </c>
       <c r="B133" s="16" t="s">
-        <v>510</v>
+        <v>506</v>
       </c>
       <c r="C133" s="84">
         <v>216422</v>
@@ -23863,7 +23860,7 @@
         <v>58820</v>
       </c>
       <c r="B134" s="16" t="s">
-        <v>511</v>
+        <v>507</v>
       </c>
       <c r="C134" s="84">
         <v>4355</v>
@@ -23901,7 +23898,7 @@
         <v>58890</v>
       </c>
       <c r="B135" s="16" t="s">
-        <v>512</v>
+        <v>508</v>
       </c>
       <c r="C135" s="84">
         <v>795</v>
@@ -23939,7 +23936,7 @@
         <v>59030</v>
       </c>
       <c r="B136" s="16" t="s">
-        <v>513</v>
+        <v>509</v>
       </c>
       <c r="C136" s="84">
         <v>255</v>
@@ -23977,7 +23974,7 @@
         <v>59100</v>
       </c>
       <c r="B137" s="16" t="s">
-        <v>514</v>
+        <v>510</v>
       </c>
       <c r="C137" s="84">
         <v>712</v>
@@ -24015,7 +24012,7 @@
         <v>59170</v>
       </c>
       <c r="B138" s="16" t="s">
-        <v>515</v>
+        <v>511</v>
       </c>
       <c r="C138" s="84">
         <v>1050</v>
@@ -24053,7 +24050,7 @@
         <v>59250</v>
       </c>
       <c r="B139" s="16" t="s">
-        <v>516</v>
+        <v>512</v>
       </c>
       <c r="C139" s="84">
         <v>570</v>
@@ -24091,7 +24088,7 @@
         <v>59310</v>
       </c>
       <c r="B140" s="16" t="s">
-        <v>517</v>
+        <v>513</v>
       </c>
       <c r="C140" s="84">
         <v>1336</v>
@@ -24129,7 +24126,7 @@
         <v>59320</v>
       </c>
       <c r="B141" s="16" t="s">
-        <v>518</v>
+        <v>514</v>
       </c>
       <c r="C141" s="84">
         <v>469</v>
@@ -24167,7 +24164,7 @@
         <v>59330</v>
       </c>
       <c r="B142" s="16" t="s">
-        <v>519</v>
+        <v>515</v>
       </c>
       <c r="C142" s="84">
         <v>484</v>
@@ -24205,7 +24202,7 @@
         <v>59340</v>
       </c>
       <c r="B143" s="16" t="s">
-        <v>520</v>
+        <v>516</v>
       </c>
       <c r="C143" s="84">
         <v>8050</v>
@@ -24243,7 +24240,7 @@
         <v>59350</v>
       </c>
       <c r="B144" s="16" t="s">
-        <v>521</v>
+        <v>517</v>
       </c>
       <c r="C144" s="84">
         <v>364</v>
@@ -24281,7 +24278,7 @@
         <v>59360</v>
       </c>
       <c r="B145" s="16" t="s">
-        <v>522</v>
+        <v>518</v>
       </c>
       <c r="C145" s="84">
         <v>1205</v>
@@ -24319,7 +24316,7 @@
         <v>59370</v>
       </c>
       <c r="B146" s="16" t="s">
-        <v>523</v>
+        <v>519</v>
       </c>
       <c r="C146" s="84">
         <v>3553</v>
@@ -24371,7 +24368,7 @@
     <row r="148" spans="1:27" ht="12" thickBot="1">
       <c r="A148" s="86"/>
       <c r="B148" s="86" t="s">
-        <v>571</v>
+        <v>567</v>
       </c>
       <c r="C148" s="70">
         <v>2749365</v>
@@ -24427,7 +24424,7 @@
         <v>51710</v>
       </c>
       <c r="B150" s="43" t="s">
-        <v>385</v>
+        <v>381</v>
       </c>
       <c r="C150" s="43">
         <v>1717</v>
@@ -24462,7 +24459,7 @@
         <v>51860</v>
       </c>
       <c r="B151" s="43" t="s">
-        <v>386</v>
+        <v>382</v>
       </c>
       <c r="C151">
         <v>603</v>
@@ -24500,7 +24497,7 @@
     </row>
     <row r="153" spans="1:27" s="15" customFormat="1">
       <c r="A153" s="27" t="s">
-        <v>572</v>
+        <v>568</v>
       </c>
       <c r="B153" s="60"/>
       <c r="C153" s="60"/>
@@ -24524,7 +24521,7 @@
     </row>
     <row r="156" spans="1:27" s="15" customFormat="1">
       <c r="A156" s="40" t="s">
-        <v>577</v>
+        <v>573</v>
       </c>
       <c r="B156" s="60"/>
       <c r="C156" s="60"/>
@@ -24625,7 +24622,7 @@
     </row>
     <row r="4" spans="1:14" s="23" customFormat="1" ht="20.100000000000001" customHeight="1">
       <c r="A4" s="1" t="s">
-        <v>605</v>
+        <v>601</v>
       </c>
       <c r="B4" s="62"/>
       <c r="C4" s="62"/>
@@ -24659,7 +24656,7 @@
       <c r="G6" s="102"/>
       <c r="H6" s="52"/>
       <c r="I6" s="105" t="s">
-        <v>575</v>
+        <v>571</v>
       </c>
       <c r="J6" s="105"/>
       <c r="K6" s="105"/>
@@ -24677,7 +24674,7 @@
       </c>
       <c r="E7" s="6"/>
       <c r="F7" s="103" t="s">
-        <v>592</v>
+        <v>588</v>
       </c>
       <c r="G7" s="104"/>
       <c r="H7" s="52"/>
@@ -24695,7 +24692,7 @@
         <v>6</v>
       </c>
       <c r="N7" s="29" t="s">
-        <v>576</v>
+        <v>572</v>
       </c>
     </row>
     <row r="8" spans="1:14" s="15" customFormat="1" ht="11.25" customHeight="1">
@@ -24757,7 +24754,7 @@
         <v>60210</v>
       </c>
       <c r="B10" s="16" t="s">
-        <v>524</v>
+        <v>520</v>
       </c>
       <c r="C10" s="84">
         <v>6933</v>
@@ -24795,7 +24792,7 @@
         <v>60410</v>
       </c>
       <c r="B11" s="16" t="s">
-        <v>525</v>
+        <v>521</v>
       </c>
       <c r="C11" s="84">
         <v>19261</v>
@@ -24833,7 +24830,7 @@
         <v>60610</v>
       </c>
       <c r="B12" s="16" t="s">
-        <v>526</v>
+        <v>522</v>
       </c>
       <c r="C12" s="84">
         <v>20408</v>
@@ -24871,7 +24868,7 @@
         <v>60810</v>
       </c>
       <c r="B13" s="16" t="s">
-        <v>527</v>
+        <v>523</v>
       </c>
       <c r="C13" s="84">
         <v>23258</v>
@@ -24909,7 +24906,7 @@
         <v>61010</v>
       </c>
       <c r="B14" s="16" t="s">
-        <v>528</v>
+        <v>524</v>
       </c>
       <c r="C14" s="84">
         <v>2579</v>
@@ -24947,7 +24944,7 @@
         <v>61210</v>
       </c>
       <c r="B15" s="16" t="s">
-        <v>529</v>
+        <v>525</v>
       </c>
       <c r="C15" s="84">
         <v>8325</v>
@@ -24985,7 +24982,7 @@
         <v>61410</v>
       </c>
       <c r="B16" s="16" t="s">
-        <v>530</v>
+        <v>526</v>
       </c>
       <c r="C16" s="84">
         <v>62336</v>
@@ -25023,7 +25020,7 @@
         <v>61510</v>
       </c>
       <c r="B17" s="16" t="s">
-        <v>531</v>
+        <v>527</v>
       </c>
       <c r="C17" s="84">
         <v>11106</v>
@@ -25061,7 +25058,7 @@
         <v>61610</v>
       </c>
       <c r="B18" s="16" t="s">
-        <v>532</v>
+        <v>528</v>
       </c>
       <c r="C18" s="84">
         <v>26896</v>
@@ -25099,7 +25096,7 @@
         <v>61810</v>
       </c>
       <c r="B19" s="16" t="s">
-        <v>533</v>
+        <v>529</v>
       </c>
       <c r="C19" s="84">
         <v>6983</v>
@@ -25137,7 +25134,7 @@
         <v>62010</v>
       </c>
       <c r="B20" s="16" t="s">
-        <v>534</v>
+        <v>530</v>
       </c>
       <c r="C20" s="84">
         <v>938</v>
@@ -25175,7 +25172,7 @@
         <v>62210</v>
       </c>
       <c r="B21" s="16" t="s">
-        <v>535</v>
+        <v>531</v>
       </c>
       <c r="C21" s="84">
         <v>7206</v>
@@ -25213,7 +25210,7 @@
         <v>62410</v>
       </c>
       <c r="B22" s="16" t="s">
-        <v>536</v>
+        <v>532</v>
       </c>
       <c r="C22" s="84">
         <v>5113</v>
@@ -25251,7 +25248,7 @@
         <v>62610</v>
       </c>
       <c r="B23" s="16" t="s">
-        <v>537</v>
+        <v>533</v>
       </c>
       <c r="C23" s="84">
         <v>51159</v>
@@ -25289,7 +25286,7 @@
         <v>62810</v>
       </c>
       <c r="B24" s="16" t="s">
-        <v>538</v>
+        <v>534</v>
       </c>
       <c r="C24" s="84">
         <v>55947</v>
@@ -25327,7 +25324,7 @@
         <v>63010</v>
       </c>
       <c r="B25" s="16" t="s">
-        <v>539</v>
+        <v>535</v>
       </c>
       <c r="C25" s="84">
         <v>18797</v>
@@ -25365,7 +25362,7 @@
         <v>63210</v>
       </c>
       <c r="B26" s="16" t="s">
-        <v>540</v>
+        <v>536</v>
       </c>
       <c r="C26" s="84">
         <v>6775</v>
@@ -25403,7 +25400,7 @@
         <v>63410</v>
       </c>
       <c r="B27" s="16" t="s">
-        <v>541</v>
+        <v>537</v>
       </c>
       <c r="C27" s="84">
         <v>1652</v>
@@ -25441,7 +25438,7 @@
         <v>63610</v>
       </c>
       <c r="B28" s="16" t="s">
-        <v>542</v>
+        <v>538</v>
       </c>
       <c r="C28" s="84">
         <v>40769</v>
@@ -25479,7 +25476,7 @@
         <v>63810</v>
       </c>
       <c r="B29" s="16" t="s">
-        <v>543</v>
+        <v>539</v>
       </c>
       <c r="C29" s="84">
         <v>12697</v>
@@ -25517,7 +25514,7 @@
         <v>64010</v>
       </c>
       <c r="B30" s="16" t="s">
-        <v>544</v>
+        <v>540</v>
       </c>
       <c r="C30" s="84">
         <v>71788</v>
@@ -25555,7 +25552,7 @@
         <v>64210</v>
       </c>
       <c r="B31" s="16" t="s">
-        <v>545</v>
+        <v>541</v>
       </c>
       <c r="C31" s="84">
         <v>21139</v>
@@ -25593,7 +25590,7 @@
         <v>64610</v>
       </c>
       <c r="B32" s="16" t="s">
-        <v>546</v>
+        <v>542</v>
       </c>
       <c r="C32" s="84">
         <v>14022</v>
@@ -25631,7 +25628,7 @@
         <v>64810</v>
       </c>
       <c r="B33" s="16" t="s">
-        <v>547</v>
+        <v>543</v>
       </c>
       <c r="C33" s="84">
         <v>16963</v>
@@ -25669,7 +25666,7 @@
         <v>65010</v>
       </c>
       <c r="B34" s="16" t="s">
-        <v>548</v>
+        <v>544</v>
       </c>
       <c r="C34" s="84">
         <v>6834</v>
@@ -25707,7 +25704,7 @@
         <v>65210</v>
       </c>
       <c r="B35" s="16" t="s">
-        <v>549</v>
+        <v>545</v>
       </c>
       <c r="C35" s="84">
         <v>2643</v>
@@ -25745,7 +25742,7 @@
         <v>65410</v>
       </c>
       <c r="B36" s="16" t="s">
-        <v>550</v>
+        <v>546</v>
       </c>
       <c r="C36" s="84">
         <v>14629</v>
@@ -25783,7 +25780,7 @@
         <v>65610</v>
       </c>
       <c r="B37" s="16" t="s">
-        <v>551</v>
+        <v>547</v>
       </c>
       <c r="C37" s="84">
         <v>4366</v>
@@ -25821,7 +25818,7 @@
         <v>65810</v>
       </c>
       <c r="B38" s="16" t="s">
-        <v>552</v>
+        <v>548</v>
       </c>
       <c r="C38" s="84">
         <v>25717</v>
@@ -25921,7 +25918,7 @@
     </row>
     <row r="43" spans="1:14" s="15" customFormat="1">
       <c r="A43" s="40" t="s">
-        <v>577</v>
+        <v>573</v>
       </c>
       <c r="B43" s="60"/>
       <c r="C43" s="60"/>
@@ -26022,7 +26019,7 @@
     </row>
     <row r="4" spans="1:14" s="23" customFormat="1" ht="20.100000000000001" customHeight="1">
       <c r="A4" s="1" t="s">
-        <v>606</v>
+        <v>602</v>
       </c>
       <c r="B4" s="62"/>
       <c r="C4" s="62"/>
@@ -26056,7 +26053,7 @@
       <c r="G6" s="102"/>
       <c r="H6" s="52"/>
       <c r="I6" s="105" t="s">
-        <v>575</v>
+        <v>571</v>
       </c>
       <c r="J6" s="105"/>
       <c r="K6" s="105"/>
@@ -26074,7 +26071,7 @@
       </c>
       <c r="E7" s="6"/>
       <c r="F7" s="103" t="s">
-        <v>592</v>
+        <v>588</v>
       </c>
       <c r="G7" s="104"/>
       <c r="H7" s="52"/>
@@ -26092,7 +26089,7 @@
         <v>6</v>
       </c>
       <c r="N7" s="29" t="s">
-        <v>576</v>
+        <v>572</v>
       </c>
     </row>
     <row r="8" spans="1:14" s="15" customFormat="1" ht="11.25" customHeight="1">
@@ -26154,7 +26151,7 @@
         <v>70200</v>
       </c>
       <c r="B10" s="16" t="s">
-        <v>553</v>
+        <v>549</v>
       </c>
       <c r="C10" s="84">
         <v>28483</v>
@@ -26192,7 +26189,7 @@
         <v>70420</v>
       </c>
       <c r="B11" s="16" t="s">
-        <v>554</v>
+        <v>550</v>
       </c>
       <c r="C11" s="84">
         <v>7189</v>
@@ -26230,7 +26227,7 @@
         <v>70540</v>
       </c>
       <c r="B12" s="16" t="s">
-        <v>555</v>
+        <v>551</v>
       </c>
       <c r="C12" s="84">
         <v>165</v>
@@ -26268,7 +26265,7 @@
         <v>70620</v>
       </c>
       <c r="B13" s="16" t="s">
-        <v>556</v>
+        <v>552</v>
       </c>
       <c r="C13" s="84">
         <v>4118</v>
@@ -26306,7 +26303,7 @@
         <v>70700</v>
       </c>
       <c r="B14" s="16" t="s">
-        <v>557</v>
+        <v>553</v>
       </c>
       <c r="C14" s="84">
         <v>1400</v>
@@ -26344,7 +26341,7 @@
         <v>71000</v>
       </c>
       <c r="B15" s="16" t="s">
-        <v>558</v>
+        <v>554</v>
       </c>
       <c r="C15" s="84">
         <v>84854</v>
@@ -26382,7 +26379,7 @@
         <v>71150</v>
       </c>
       <c r="B16" s="16" t="s">
-        <v>559</v>
+        <v>555</v>
       </c>
       <c r="C16" s="84">
         <v>312</v>
@@ -26420,7 +26417,7 @@
         <v>71300</v>
       </c>
       <c r="B17" s="16" t="s">
-        <v>560</v>
+        <v>556</v>
       </c>
       <c r="C17" s="84">
         <v>10089</v>
@@ -26458,7 +26455,7 @@
         <v>72200</v>
       </c>
       <c r="B18" s="16" t="s">
-        <v>561</v>
+        <v>557</v>
       </c>
       <c r="C18" s="84">
         <v>10679</v>
@@ -26496,7 +26493,7 @@
         <v>72300</v>
       </c>
       <c r="B19" s="16" t="s">
-        <v>562</v>
+        <v>558</v>
       </c>
       <c r="C19" s="84">
         <v>22879</v>
@@ -26534,7 +26531,7 @@
         <v>72330</v>
       </c>
       <c r="B20" s="16" t="s">
-        <v>563</v>
+        <v>559</v>
       </c>
       <c r="C20" s="84">
         <v>6574</v>
@@ -26572,7 +26569,7 @@
         <v>72800</v>
       </c>
       <c r="B21" s="16" t="s">
-        <v>564</v>
+        <v>560</v>
       </c>
       <c r="C21" s="84">
         <v>39530</v>
@@ -26610,7 +26607,7 @@
         <v>73600</v>
       </c>
       <c r="B22" s="16" t="s">
-        <v>565</v>
+        <v>561</v>
       </c>
       <c r="C22" s="84">
         <v>7435</v>
@@ -26648,7 +26645,7 @@
         <v>74050</v>
       </c>
       <c r="B23" s="16" t="s">
-        <v>566</v>
+        <v>562</v>
       </c>
       <c r="C23" s="84">
         <v>2735</v>
@@ -26686,7 +26683,7 @@
         <v>74550</v>
       </c>
       <c r="B24" s="16" t="s">
-        <v>567</v>
+        <v>563</v>
       </c>
       <c r="C24" s="84">
         <v>3221</v>
@@ -26724,7 +26721,7 @@
         <v>74560</v>
       </c>
       <c r="B25" s="16" t="s">
-        <v>568</v>
+        <v>564</v>
       </c>
       <c r="C25" s="84">
         <v>464</v>
@@ -26762,7 +26759,7 @@
         <v>74660</v>
       </c>
       <c r="B26" s="16" t="s">
-        <v>569</v>
+        <v>565</v>
       </c>
       <c r="C26" s="84">
         <v>7182</v>
@@ -26800,7 +26797,7 @@
         <v>74680</v>
       </c>
       <c r="B27" s="16" t="s">
-        <v>570</v>
+        <v>566</v>
       </c>
       <c r="C27" s="84">
         <v>3422</v>
@@ -26954,7 +26951,7 @@
     </row>
     <row r="34" spans="1:14" s="15" customFormat="1">
       <c r="A34" s="40" t="s">
-        <v>577</v>
+        <v>573</v>
       </c>
       <c r="B34" s="60"/>
       <c r="C34" s="60"/>
@@ -27053,7 +27050,7 @@
     </row>
     <row r="4" spans="1:13" s="23" customFormat="1" ht="20.100000000000001" customHeight="1">
       <c r="A4" s="1" t="s">
-        <v>607</v>
+        <v>603</v>
       </c>
       <c r="F4" s="53"/>
       <c r="G4" s="53"/>
@@ -27083,7 +27080,7 @@
       <c r="F6" s="102"/>
       <c r="G6" s="52"/>
       <c r="H6" s="105" t="s">
-        <v>575</v>
+        <v>571</v>
       </c>
       <c r="I6" s="105"/>
       <c r="J6" s="105"/>
@@ -27100,7 +27097,7 @@
       </c>
       <c r="D7" s="6"/>
       <c r="E7" s="103" t="s">
-        <v>592</v>
+        <v>588</v>
       </c>
       <c r="F7" s="104"/>
       <c r="G7" s="52"/>
@@ -27118,7 +27115,7 @@
         <v>6</v>
       </c>
       <c r="M7" s="29" t="s">
-        <v>576</v>
+        <v>572</v>
       </c>
     </row>
     <row r="8" spans="1:13" s="15" customFormat="1" ht="11.25" customHeight="1">
@@ -27560,7 +27557,7 @@
     </row>
     <row r="23" spans="1:13" s="15" customFormat="1">
       <c r="A23" s="40" t="s">
-        <v>577</v>
+        <v>573</v>
       </c>
       <c r="B23" s="60"/>
       <c r="C23" s="60"/>

</xml_diff>